<commit_message>
Added my tests and updated my user story again
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
+++ b/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedlehr/Documents/Texas State/CS3398/2018 Fall/Assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23460" windowHeight="12120" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23460" windowHeight="12120" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="How to use this template" sheetId="5" r:id="rId1"/>
@@ -18,11 +18,8 @@
     <sheet name="Test Creation Assigments" sheetId="3" r:id="rId4"/>
     <sheet name="Test Data" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36,7 +33,7 @@
     <author>Clint Tuttle</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="100">
   <si>
     <t>Creator</t>
   </si>
@@ -212,15 +209,6 @@
   </si>
   <si>
     <t>Passed</t>
-  </si>
-  <si>
-    <t>Test 4</t>
-  </si>
-  <si>
-    <t>Actual results of failure and detail on how to recreate if needed</t>
-  </si>
-  <si>
-    <t>Test 5</t>
   </si>
   <si>
     <t>Test 6</t>
@@ -334,28 +322,6 @@
     <t xml:space="preserve">Feel free to organize the information on this page so that it is most efficient and intuitive for the testers to find and use during testing. </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Refer to </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>filename</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> for documentation</t>
-    </r>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -365,15 +331,6 @@
     <t>Actual Test Date</t>
   </si>
   <si>
-    <t>enter step here…</t>
-  </si>
-  <si>
-    <t>Test 2 Description</t>
-  </si>
-  <si>
-    <t>Test 3 …</t>
-  </si>
-  <si>
     <t>Executed Steps</t>
   </si>
   <si>
@@ -420,13 +377,67 @@
   </si>
   <si>
     <t>Class:  RaBoof</t>
+  </si>
+  <si>
+    <t>User Story 1: Joel</t>
+  </si>
+  <si>
+    <t>Bot will detect subscription</t>
+  </si>
+  <si>
+    <t>Run bot on a popular Twitch channel</t>
+  </si>
+  <si>
+    <t>Bot connects to specified channel</t>
+  </si>
+  <si>
+    <t>Some user subscribes to the streamer</t>
+  </si>
+  <si>
+    <t>The message "/*/*/*/*/*Subscriber has been detected/*/*/*/*/*" will appear on the node.js command window</t>
+  </si>
+  <si>
+    <t>Joel</t>
+  </si>
+  <si>
+    <t>Bot will ignore chat message posing as a sub alert</t>
+  </si>
+  <si>
+    <t>Run bot on a channel</t>
+  </si>
+  <si>
+    <t>User types "/*/*/*/*/*Subscriber has been detected/*/*/*/*/*"</t>
+  </si>
+  <si>
+    <t>No sub detection message should appear in the node.js command window</t>
+  </si>
+  <si>
+    <t>User Story 2: Joel</t>
+  </si>
+  <si>
+    <t>User inputs !gamble command incorrectly</t>
+  </si>
+  <si>
+    <t>User types in "!gamble blah"</t>
+  </si>
+  <si>
+    <t>Bot should say 'You did not enter either tails or heads loser...smh'</t>
+  </si>
+  <si>
+    <t>User uses !gamble</t>
+  </si>
+  <si>
+    <t>User type in either "!gamble heads" or "!gamble tails"</t>
+  </si>
+  <si>
+    <t>Bot will either say that the user lost or won a number of points.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -465,12 +476,6 @@
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -505,7 +510,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -715,11 +720,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -797,13 +811,38 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1091,43 +1130,43 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="118" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="42" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="41"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="41"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" s="12"/>
     </row>
   </sheetData>
@@ -1139,67 +1178,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" customWidth="1"/>
-    <col min="4" max="4" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C5" s="22">
         <f>COUNT('Test Case Tracker'!B:B)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="24">
         <f>COUNTA('Test Case Tracker'!D:D)-1</f>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="27"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="30" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C9" s="20">
         <f>C7-C11</f>
@@ -1207,47 +1246,47 @@
       </c>
       <c r="D9" s="31">
         <f>C9/C7</f>
-        <v>0.48148148148148145</v>
+        <v>0.5</v>
       </c>
       <c r="E9" s="29"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="32"/>
       <c r="C10" s="28"/>
       <c r="D10" s="31"/>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="30" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C11" s="20">
         <f>SUM(C12:C13)</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="31">
         <f>C11/C7</f>
-        <v>0.51851851851851849</v>
+        <v>0.5</v>
       </c>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="33" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="20">
         <f>COUNTIF('Test Case Tracker'!G:G,B12)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="31">
         <f>C12/C11</f>
-        <v>0.7857142857142857</v>
+        <v>0.76923076923076927</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="35" t="s">
         <v>25</v>
       </c>
@@ -1257,22 +1296,22 @@
       </c>
       <c r="D13" s="37">
         <f>C13/C11</f>
-        <v>0.21428571428571427</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D15" s="8"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1283,28 +1322,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" customWidth="1"/>
-    <col min="6" max="6" width="45" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="39.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+    <col min="6" max="6" width="50.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" customWidth="1"/>
     <col min="9" max="9" width="16" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>2</v>
@@ -1313,7 +1352,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>8</v>
@@ -1328,27 +1367,27 @@
         <v>11</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J1" s="16" t="s">
         <v>12</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" s="18">
         <v>1</v>
@@ -1364,16 +1403,16 @@
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="14"/>
@@ -1391,76 +1430,74 @@
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="19">
+    <row r="4" spans="1:12" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="46">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="I4" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K4" s="51"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="D5" s="18">
         <v>1</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>56</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="J5" s="6"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="15"/>
@@ -1468,181 +1505,167 @@
         <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>56</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="J6" s="6"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="19">
+        <v>82</v>
+      </c>
+      <c r="B7" s="3">
         <v>3</v>
       </c>
+      <c r="C7" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1</v>
+      </c>
       <c r="E7" s="5" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>56</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="J7" s="6"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="15"/>
       <c r="D8" s="19">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="3">
         <v>4</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="3">
-        <v>3</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="18">
+      <c r="C9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="19">
         <v>1</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>33</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="J9" s="9"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>59</v>
+    <row r="10" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="39" t="s">
+        <v>93</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="15"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="19">
         <v>2</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="H10" s="5"/>
       <c r="I10" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="J10" s="9"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="B11" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="D11" s="19">
         <v>1</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="H11" s="5"/>
       <c r="I11" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>55</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="J11" s="9"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="B12" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" s="19">
         <v>1</v>
@@ -1660,22 +1683,22 @@
         <v>32</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B13" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" s="19">
         <v>1</v>
@@ -1693,22 +1716,23 @@
         <v>32</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B14" s="3">
-        <v>7</v>
+        <f t="shared" ref="B14:B27" si="0">B13+1</f>
+        <v>8</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" s="19">
         <v>1</v>
@@ -1726,23 +1750,23 @@
         <v>32</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>4</v>
+        <v>53</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" ref="B15:B28" si="0">B14+1</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="19">
         <v>1</v>
@@ -1753,30 +1777,28 @@
       <c r="F15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="G15" s="4"/>
       <c r="H15" s="5" t="s">
         <v>32</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B16" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="19">
         <v>1</v>
@@ -1795,20 +1817,20 @@
         <v>4</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B17" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="19">
         <v>1</v>
@@ -1824,23 +1846,23 @@
         <v>32</v>
       </c>
       <c r="I17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="9" t="s">
-        <v>55</v>
-      </c>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B18" s="3">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" s="19">
         <v>1</v>
@@ -1856,23 +1878,23 @@
         <v>32</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B19" s="3">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D19" s="19">
         <v>1</v>
@@ -1888,23 +1910,23 @@
         <v>32</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D20" s="19">
         <v>1</v>
@@ -1920,23 +1942,23 @@
         <v>32</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="J20" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="J20" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21" s="19">
         <v>1</v>
@@ -1952,23 +1974,23 @@
         <v>32</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" s="3">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D22" s="19">
         <v>1</v>
@@ -1984,23 +2006,23 @@
         <v>32</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23" s="3">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D23" s="19">
         <v>1</v>
@@ -2016,23 +2038,23 @@
         <v>32</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B24" s="3">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" s="19">
         <v>1</v>
@@ -2048,23 +2070,23 @@
         <v>32</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B25" s="3">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D25" s="19">
         <v>1</v>
@@ -2080,23 +2102,23 @@
         <v>32</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B26" s="3">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D26" s="19">
         <v>1</v>
@@ -2112,23 +2134,23 @@
         <v>32</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B27" s="3">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D27" s="19">
         <v>1</v>
@@ -2144,53 +2166,22 @@
         <v>32</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="3">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="19">
-        <v>1</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K28" s="7"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="G2:G28">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G27">
       <formula1>"Passed,Failed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2202,9 +2193,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2212,7 +2203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2220,28 +2211,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2257,24 +2248,24 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2285,7 +2276,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -2296,7 +2287,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Did my user stories for testing
bleh bleh bleh bleh bleh
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
+++ b/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{548BB185-17BF-436C-A68E-CF7AEDE8FEF5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="23460" windowHeight="12120" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23460" windowHeight="12120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use this template" sheetId="5" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Test Creation Assigments" sheetId="3" r:id="rId4"/>
     <sheet name="Test Data" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Clint Tuttle</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -89,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="106">
   <si>
     <t>Creator</t>
   </si>
@@ -148,12 +149,6 @@
     <t>Tested By</t>
   </si>
   <si>
-    <t>Navigate to website.com</t>
-  </si>
-  <si>
-    <t>User will see homepage of website.com</t>
-  </si>
-  <si>
     <t>Scenarios</t>
   </si>
   <si>
@@ -166,18 +161,6 @@
     <t>invalid user</t>
   </si>
   <si>
-    <t>Click Login button in top right corner</t>
-  </si>
-  <si>
-    <t>User is navigated a login screen</t>
-  </si>
-  <si>
-    <t>Enter "admin" in username column and "password1" in password box.  Click Login button.</t>
-  </si>
-  <si>
-    <t>User will receive the following error: "Please enter a valid username/password"</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -190,9 +173,6 @@
     <t>valid user</t>
   </si>
   <si>
-    <t>Error message was a cryptic java error message</t>
-  </si>
-  <si>
     <t>admin-test</t>
   </si>
   <si>
@@ -271,25 +251,7 @@
     <t>Joe</t>
   </si>
   <si>
-    <t>Login with incorrect password</t>
-  </si>
-  <si>
     <t>User Story</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">User Story 1: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Name</t>
-    </r>
   </si>
   <si>
     <r>
@@ -432,11 +394,56 @@
   <si>
     <t>Bot will either say that the user lost or won a number of points.</t>
   </si>
+  <si>
+    <t>User Story 1: !slap</t>
+  </si>
+  <si>
+    <t>User Story 1: !stats</t>
+  </si>
+  <si>
+    <t>Levi: Bot will slap either a random, or a specified user.</t>
+  </si>
+  <si>
+    <t>Run bot on channel</t>
+  </si>
+  <si>
+    <t>Bot connects, shown on console log</t>
+  </si>
+  <si>
+    <t>bot puts "[username] You have been slapped!" in chat</t>
+  </si>
+  <si>
+    <t>bot puts "[randomuser] You have been Slapped!" in chat</t>
+  </si>
+  <si>
+    <t>bot puts"[username] is not in chat" in chat</t>
+  </si>
+  <si>
+    <t>Levi: Bot will return user status information</t>
+  </si>
+  <si>
+    <t>User writes"!stats" in chat</t>
+  </si>
+  <si>
+    <t>User writes "!slap" in chat</t>
+  </si>
+  <si>
+    <t>User writes "!slap [username]" in chat</t>
+  </si>
+  <si>
+    <t>User writes "!slap [username]" in chat, and [username is not in chat</t>
+  </si>
+  <si>
+    <t>Bot puts user information in chat</t>
+  </si>
+  <si>
+    <t>Levi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -733,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -820,28 +827,22 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1123,7 +1124,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
@@ -1137,27 +1138,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="42" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
@@ -1175,7 +1176,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1191,29 +1192,29 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C5" s="22">
         <f>COUNT('Test Case Tracker'!B:B)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1225,7 +1226,7 @@
       </c>
       <c r="C7" s="24">
         <f>COUNTA('Test Case Tracker'!D:D)-1</f>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -1238,7 +1239,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="30" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C9" s="20">
         <f>C7-C11</f>
@@ -1246,7 +1247,7 @@
       </c>
       <c r="D9" s="31">
         <f>C9/C7</f>
-        <v>0.5</v>
+        <v>0.44827586206896552</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -1258,48 +1259,48 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="30" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C11" s="20">
         <f>SUM(C12:C13)</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D11" s="31">
         <f>C11/C7</f>
-        <v>0.5</v>
+        <v>0.55172413793103448</v>
       </c>
       <c r="E11" s="29"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="33" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C12" s="20">
         <f>COUNTIF('Test Case Tracker'!G:G,B12)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D12" s="31">
         <f>C12/C11</f>
-        <v>0.76923076923076927</v>
+        <v>0.9375</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C13" s="36">
         <f>COUNTIF('Test Case Tracker'!G:G,B13)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" s="37">
         <f>C13/C11</f>
-        <v>0.23076923076923078</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1311,7 +1312,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1321,18 +1322,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.28515625" customWidth="1"/>
     <col min="6" max="6" width="50.140625" customWidth="1"/>
@@ -1341,9 +1342,9 @@
     <col min="9" max="9" width="16" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>2</v>
@@ -1352,7 +1353,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>8</v>
@@ -1367,52 +1368,50 @@
         <v>11</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J1" s="16" t="s">
         <v>12</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="D2" s="18">
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="14"/>
@@ -1420,721 +1419,699 @@
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:20" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="18">
+        <v>3</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="45"/>
+      <c r="I4" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" s="48"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+    </row>
+    <row r="5" spans="1:20" s="28" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="18">
         <v>4</v>
       </c>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46">
-        <v>3</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="51"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="E5" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="I5" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" s="48"/>
+      <c r="K5" s="49"/>
+    </row>
+    <row r="6" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="18">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="19">
-        <v>2</v>
+      <c r="C6" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="18">
+        <v>1</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="9" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L6"/>
+    </row>
+    <row r="7" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="3">
-        <v>3</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="18">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="19">
+        <v>2</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="9" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L7"/>
+    </row>
+    <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="19">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="18">
+        <v>1</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>94</v>
-      </c>
+    <row r="9" spans="1:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="J9" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="J9" s="6"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="19">
-        <v>2</v>
+    <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="3">
+        <v>4</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="18">
+        <v>1</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="J10" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="J10" s="6"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="3">
-        <v>5</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>97</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="19">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="19">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="3">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="3">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="19">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="6" t="s">
+      <c r="D14" s="19">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="19">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="3">
-        <v>7</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="19">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="J13" s="6" t="s">
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="3">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="19">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="3">
-        <f t="shared" ref="B14:B27" si="0">B13+1</f>
-        <v>8</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="19">
-        <v>1</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K14" s="7"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="19">
-        <v>1</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K15" s="7"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="19">
-        <v>1</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D17" s="19">
         <v>1</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H17" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>4</v>
+        <v>46</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D18" s="19">
         <v>1</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="K18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D19" s="19">
         <v>1</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B20" s="3">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D20" s="19">
         <v>1</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D21" s="19">
         <v>1</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D22" s="19">
         <v>1</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D23" s="19">
         <v>1</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="6" t="s">
         <v>4</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B24" s="3">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D24" s="19">
         <v>1</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>4</v>
+        <v>45</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B25" s="3">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D25" s="19">
         <v>1</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>4</v>
+        <v>44</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B26" s="3">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D26" s="19">
         <v>1</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>4</v>
@@ -2143,39 +2120,131 @@
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B27" s="3">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D27" s="19">
         <v>1</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K27" s="7"/>
     </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="3">
+        <v>20</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="19">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="3">
+        <v>21</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="19">
+        <v>1</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="3">
+        <v>22</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="19">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="7"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="G2:G27">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G30" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Passed,Failed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2186,7 +2255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2213,7 +2282,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -2221,18 +2290,18 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2241,7 +2310,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2252,50 +2321,50 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I think I'm done? tell me If i'm stupid
Do check that I'm not stupid please
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
+++ b/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{548BB185-17BF-436C-A68E-CF7AEDE8FEF5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E27BCF04-33C6-4FCB-B679-A44EB8BEF3BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="23460" windowHeight="12120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,6 +29,85 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Clint Tuttle</author>
+  </authors>
+  <commentList>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{1EEF4434-2D00-4755-A0E9-5904BB6D5651}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">List number on first step of each unique test case so we can count # of total test cases	
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{1D638DA9-742C-424F-9FF8-EB48340C832A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Describe the purpose of the overall test case	
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{980F5856-F51B-48CF-8105-A075A0827717}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Be descriptive enough so anyone could follow the step and not need prior knowledge of system to run it	
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{F49E239A-31C0-4032-982E-9529E66E4A9C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Ensure results are clear and not vague
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{88ECEABC-3C52-4F04-9D75-ED110DB6FFA5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Make sure you designate each step as either "passed" (i.e. worked as expected) or "failed" (i.e. didn't work as expected).  You need to pass or fail each step to ensure execution % calculates correctly.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Clint Tuttle</author>
@@ -108,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="108">
   <si>
     <t>Creator</t>
   </si>
@@ -218,27 +297,6 @@
     <t>Test 14</t>
   </si>
   <si>
-    <t>Test 15</t>
-  </si>
-  <si>
-    <t>Test 16</t>
-  </si>
-  <si>
-    <t>Test 17</t>
-  </si>
-  <si>
-    <t>Test 18</t>
-  </si>
-  <si>
-    <t>Test 19</t>
-  </si>
-  <si>
-    <t>Test 20</t>
-  </si>
-  <si>
-    <t>Test 21</t>
-  </si>
-  <si>
     <t>Written By</t>
   </si>
   <si>
@@ -254,21 +312,6 @@
     <t>User Story</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">User Story 2: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Name</t>
-    </r>
-  </si>
-  <si>
     <t>Testing Status Dashboard</t>
   </si>
   <si>
@@ -438,6 +481,36 @@
   </si>
   <si>
     <t>Levi</t>
+  </si>
+  <si>
+    <t>User Story 3: !slap</t>
+  </si>
+  <si>
+    <t>User Story 3: !stats</t>
+  </si>
+  <si>
+    <t>Class:  slap</t>
+  </si>
+  <si>
+    <t>Class:  stats</t>
+  </si>
+  <si>
+    <t>Levi: Test 18</t>
+  </si>
+  <si>
+    <t>Levi: Test 19</t>
+  </si>
+  <si>
+    <t>Levi: Test 20</t>
+  </si>
+  <si>
+    <t>Levi: Test 21</t>
+  </si>
+  <si>
+    <t>Levi: Test 16</t>
+  </si>
+  <si>
+    <t>Levi: Test 17</t>
   </si>
 </sst>
 </file>
@@ -1124,11 +1197,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="J21" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="W33" sqref="N24:W33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1136,42 +1209,956 @@
     <col min="1" max="1" width="118" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="3">
+        <v>1</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q2" s="18">
+        <v>1</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="5"/>
+      <c r="V2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="W2" s="6"/>
+    </row>
+    <row r="3" spans="1:23" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" t="s">
+        <v>83</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="19">
+        <v>2</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="5"/>
+      <c r="V3" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="W3" s="6"/>
+    </row>
+    <row r="4" spans="1:23" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="O4" s="44"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="18">
+        <v>3</v>
+      </c>
+      <c r="R4" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="S4" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="T4" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="45"/>
+      <c r="V4" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="W4" s="48"/>
+    </row>
+    <row r="5" spans="1:23" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="O5" s="44"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="18">
+        <v>4</v>
+      </c>
+      <c r="R5" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="S5" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="T5" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="U5" s="45"/>
+      <c r="V5" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="W5" s="48"/>
+    </row>
+    <row r="6" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="41"/>
+      <c r="N6" t="s">
+        <v>84</v>
+      </c>
+      <c r="O6" s="3">
+        <v>2</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>1</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U6" s="5"/>
+      <c r="V6" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="W6" s="6"/>
+    </row>
+    <row r="7" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="41"/>
+      <c r="N7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O7" s="3"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="19">
+        <v>2</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U7" s="5"/>
+      <c r="V7" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="W7" s="6"/>
+    </row>
+    <row r="8" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>65</v>
+      </c>
+      <c r="O8" s="3">
+        <v>3</v>
+      </c>
+      <c r="P8" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>1</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="5"/>
+      <c r="V8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="W8" s="6"/>
+    </row>
+    <row r="9" spans="1:23" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>65</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="19">
+        <v>2</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U9" s="5"/>
+      <c r="V9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="W9" s="6"/>
+    </row>
+    <row r="10" spans="1:23" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>65</v>
+      </c>
+      <c r="O10" s="3">
+        <v>4</v>
+      </c>
+      <c r="P10" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q10" s="18">
+        <v>1</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U10" s="5"/>
+      <c r="V10" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="W10" s="6"/>
+    </row>
+    <row r="11" spans="1:23" ht="102" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O11" s="3"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="19">
+        <v>2</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U11" s="5"/>
+      <c r="V11" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="W11" s="6"/>
+    </row>
+    <row r="12" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="N12" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="O12" s="3">
+        <v>5</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>1</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U12" s="5"/>
+      <c r="V12" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="W12" s="9"/>
+    </row>
+    <row r="13" spans="1:23" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="N13" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="3"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="19">
+        <v>2</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U13" s="5"/>
+      <c r="V13" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="W13" s="9"/>
+    </row>
+    <row r="14" spans="1:23" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="N14" t="s">
+        <v>76</v>
+      </c>
+      <c r="O14" s="3">
+        <v>6</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q14" s="19">
+        <v>1</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U14" s="5"/>
+      <c r="V14" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="W14" s="9"/>
+    </row>
+    <row r="15" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="N15" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" s="3">
+        <v>7</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="19">
+        <v>1</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="W15" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="N16" t="s">
+        <v>63</v>
+      </c>
+      <c r="O16" s="3">
+        <v>8</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="19">
+        <v>1</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="N17" t="s">
+        <v>63</v>
+      </c>
+      <c r="O17" s="3">
+        <v>9</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q17" s="19">
+        <v>1</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="N18" t="s">
+        <v>63</v>
+      </c>
+      <c r="O18" s="3">
+        <v>10</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q18" s="19">
+        <v>1</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T18" s="4"/>
+      <c r="U18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="W18" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>63</v>
+      </c>
+      <c r="O19" s="3">
+        <v>11</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q19" s="19">
+        <v>1</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T19" s="4"/>
+      <c r="U19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="W19" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="N20" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="41"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="41"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="O20" s="3">
+        <v>12</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q20" s="19">
+        <v>1</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T20" s="4"/>
+      <c r="U20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="W20" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="N21" t="s">
+        <v>64</v>
+      </c>
+      <c r="O21" s="3">
+        <v>13</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q21" s="19">
+        <v>1</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T21" s="4"/>
+      <c r="U21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="W21" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="N22" t="s">
+        <v>64</v>
+      </c>
+      <c r="O22" s="3">
+        <v>14</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q22" s="19">
+        <v>1</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T22" s="4"/>
+      <c r="U22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="W22" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="N23" t="s">
+        <v>64</v>
+      </c>
+      <c r="O23" s="3">
+        <v>15</v>
+      </c>
+      <c r="P23" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q23" s="19">
+        <v>1</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T23" s="4"/>
+      <c r="U23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V23" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="W23" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="N24" t="s">
+        <v>98</v>
+      </c>
+      <c r="O24" s="3">
+        <v>16</v>
+      </c>
+      <c r="P24" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q24" s="18">
+        <v>1</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="S24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U24" s="5"/>
+      <c r="V24" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="W24" s="6"/>
+    </row>
+    <row r="25" spans="2:23" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="N25" t="s">
+        <v>98</v>
+      </c>
+      <c r="O25" s="3"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="19">
+        <v>2</v>
+      </c>
+      <c r="R25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="S25" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U25" s="5"/>
+      <c r="V25" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="W25" s="6"/>
+    </row>
+    <row r="26" spans="2:23" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="N26" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="O26" s="44"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="18">
+        <v>3</v>
+      </c>
+      <c r="R26" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="S26" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="T26" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="U26" s="45"/>
+      <c r="V26" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="W26" s="48"/>
+    </row>
+    <row r="27" spans="2:23" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="N27" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="O27" s="44"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="18">
+        <v>4</v>
+      </c>
+      <c r="R27" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="S27" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="T27" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="U27" s="45"/>
+      <c r="V27" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="W27" s="48"/>
+    </row>
+    <row r="28" spans="2:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="N28" t="s">
+        <v>99</v>
+      </c>
+      <c r="O28" s="3">
+        <v>17</v>
+      </c>
+      <c r="P28" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q28" s="18">
+        <v>1</v>
+      </c>
+      <c r="R28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="S28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="T28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U28" s="5"/>
+      <c r="V28" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="W28" s="6"/>
+    </row>
+    <row r="29" spans="2:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="N29" t="s">
+        <v>99</v>
+      </c>
+      <c r="O29" s="3"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="19">
+        <v>2</v>
+      </c>
+      <c r="R29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="S29" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="T29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U29" s="5"/>
+      <c r="V29" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="W29" s="6"/>
+    </row>
+    <row r="30" spans="2:23" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B30" s="12"/>
+      <c r="N30" t="s">
+        <v>100</v>
+      </c>
+      <c r="O30" s="3">
+        <v>18</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q30" s="19">
+        <v>1</v>
+      </c>
+      <c r="R30" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="S30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="T30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="W30" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="N31" t="s">
+        <v>100</v>
+      </c>
+      <c r="O31" s="3">
+        <v>19</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q31" s="19">
+        <v>1</v>
+      </c>
+      <c r="R31" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="S31" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V31" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="W31" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:23" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="N32" t="s">
+        <v>100</v>
+      </c>
+      <c r="O32" s="3">
+        <v>20</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q32" s="19">
+        <v>1</v>
+      </c>
+      <c r="R32" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="S32" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="T32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V32" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="W32" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="14:23" ht="51" x14ac:dyDescent="0.2">
+      <c r="N33" t="s">
+        <v>101</v>
+      </c>
+      <c r="O33" s="3">
+        <v>21</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q33" s="19">
+        <v>1</v>
+      </c>
+      <c r="R33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="S33" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V33" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="W33" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="T2:T33" xr:uid="{78B1D5D1-D291-4BF8-8527-AFE85CD03A19}">
+      <formula1>"Passed,Failed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1192,29 +2179,29 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C5" s="22">
         <f>COUNT('Test Case Tracker'!B:B)</f>
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1226,7 +2213,7 @@
       </c>
       <c r="C7" s="24">
         <f>COUNTA('Test Case Tracker'!D:D)-1</f>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
@@ -1239,15 +2226,15 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="30" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C9" s="20">
         <f>C7-C11</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D9" s="31">
         <f>C9/C7</f>
-        <v>0.44827586206896552</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -1259,15 +2246,15 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="30" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C11" s="20">
         <f>SUM(C12:C13)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D11" s="31">
         <f>C11/C7</f>
-        <v>0.55172413793103448</v>
+        <v>0.76923076923076927</v>
       </c>
       <c r="E11" s="29"/>
     </row>
@@ -1277,14 +2264,14 @@
       </c>
       <c r="C12" s="20">
         <f>COUNTIF('Test Case Tracker'!G:G,B12)</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D12" s="31">
         <f>C12/C11</f>
-        <v>0.9375</v>
+        <v>0.95</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1297,10 +2284,10 @@
       </c>
       <c r="D13" s="37">
         <f>C13/C11</f>
-        <v>6.25E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1312,7 +2299,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1323,10 +2310,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1344,7 +2331,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>2</v>
@@ -1353,7 +2340,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>8</v>
@@ -1368,97 +2355,101 @@
         <v>11</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J1" s="16" t="s">
         <v>12</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>93</v>
+      <c r="C2" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="D2" s="18">
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="9" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="14"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="19">
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="9" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:20" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="15"/>
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>72</v>
+      </c>
       <c r="D4" s="18">
-        <v>3</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="F4" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="J4" s="48"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="28"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="K4" s="7"/>
+      <c r="L4"/>
       <c r="M4" s="28"/>
       <c r="N4" s="28"/>
       <c r="O4" s="28"/>
@@ -1469,286 +2460,317 @@
       <c r="T4" s="28"/>
     </row>
     <row r="5" spans="1:20" s="28" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="44"/>
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="15"/>
-      <c r="D5" s="18">
-        <v>4</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="J5" s="48"/>
-      <c r="K5" s="49"/>
+      <c r="D5" s="19">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="L5"/>
     </row>
     <row r="6" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>92</v>
+      <c r="A6" s="39" t="s">
+        <v>76</v>
       </c>
       <c r="B6" s="3">
-        <v>2</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="18">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="19">
         <v>1</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="J6" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="J6" s="9"/>
       <c r="K6" s="7"/>
       <c r="L6"/>
     </row>
     <row r="7" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>92</v>
+      <c r="A7" s="39" t="s">
+        <v>76</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="14"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="19">
         <v>2</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="J7" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="J7" s="9"/>
       <c r="K7" s="7"/>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B8" s="3">
-        <v>3</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="18">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="19">
         <v>1</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="J8" s="9"/>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="15"/>
+        <v>63</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D9" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="I9" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J9" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="19">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="18">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J10" s="6"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="15"/>
+        <v>63</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="D11" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>83</v>
+        <v>24</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="I11" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J11" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="39" t="s">
-        <v>84</v>
+      <c r="A12" t="s">
+        <v>63</v>
       </c>
       <c r="B12" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="D12" s="19">
         <v>1</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="I12" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3">
+        <v>9</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="D13" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="I13" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J13" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B14" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="D14" s="19">
         <v>1</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="I14" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="J14" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B15" s="3">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D15" s="19">
         <v>1</v>
@@ -1759,14 +2781,12 @@
       <c r="F15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="G15" s="4"/>
       <c r="H15" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>4</v>
@@ -1775,13 +2795,13 @@
     </row>
     <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B16" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D16" s="19">
         <v>1</v>
@@ -1792,29 +2812,27 @@
       <c r="F16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="G16" s="4"/>
       <c r="H16" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B17" s="3">
-        <v>9</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>35</v>
       </c>
       <c r="D17" s="19">
         <v>1</v>
@@ -1825,426 +2843,314 @@
       <c r="F17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="G17" s="4"/>
       <c r="H17" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="B18" s="3">
-        <v>10</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="19">
+        <v>14</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="18">
         <v>1</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="5"/>
       <c r="I18" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="18">
+        <v>3</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="45"/>
+      <c r="I20" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="J20" s="48"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="28"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="44"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="18">
         <v>4</v>
       </c>
-      <c r="J18" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K18" s="7"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="3">
-        <v>11</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" s="7"/>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="3">
-        <v>12</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="19">
-        <v>1</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="3">
-        <v>13</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="19">
-        <v>1</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K21" s="7"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="45"/>
+      <c r="I21" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="J21" s="48"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="28"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="B22" s="3">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="19">
+        <v>15</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="18">
         <v>1</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="5"/>
       <c r="I22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="J22" s="6"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="3">
-        <v>15</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="5"/>
       <c r="I23" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>46</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="J23" s="6"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="B24" s="3">
         <v>16</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="D24" s="19">
         <v>1</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="4"/>
+        <v>89</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H24" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="B25" s="3">
         <v>17</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="D25" s="19">
         <v>1</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" s="4"/>
+      <c r="E25" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H25" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="B26" s="3">
         <v>18</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>38</v>
+        <v>102</v>
       </c>
       <c r="D26" s="19">
         <v>1</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="4"/>
+      <c r="E26" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H26" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="B27" s="3">
         <v>19</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="D27" s="19">
         <v>1</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="H27" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="3">
-        <v>20</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="19">
-        <v>1</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K28" s="7"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="3">
-        <v>21</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="19">
-        <v>1</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="3">
-        <v>22</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="19">
-        <v>1</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30" s="7"/>
-    </row>
+    <row r="28" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="G2:G30" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G27" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Passed,Failed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2282,7 +3188,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -2290,18 +3196,18 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2321,17 +3227,17 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed my tests (Joel)
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
+++ b/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E27BCF04-33C6-4FCB-B679-A44EB8BEF3BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="23460" windowHeight="12120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23460" windowHeight="12120" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="How to use this template" sheetId="5" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Test Creation Assigments" sheetId="3" r:id="rId4"/>
     <sheet name="Test Data" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,12 +28,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Clint Tuttle</author>
   </authors>
   <commentList>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{1EEF4434-2D00-4755-A0E9-5904BB6D5651}">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{1D638DA9-742C-424F-9FF8-EB48340C832A}">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{980F5856-F51B-48CF-8105-A075A0827717}">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{F49E239A-31C0-4032-982E-9529E66E4A9C}">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -90,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{88ECEABC-3C52-4F04-9D75-ED110DB6FFA5}">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,12 +107,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Clint Tuttle</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -187,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="128">
   <si>
     <t>Creator</t>
   </si>
@@ -511,12 +510,72 @@
   </si>
   <si>
     <t>Levi: Test 17</t>
+  </si>
+  <si>
+    <t>Joel: Bot will detect subscription</t>
+  </si>
+  <si>
+    <t>User Story 1: onSubHandler</t>
+  </si>
+  <si>
+    <t>User Story 2: !gamble</t>
+  </si>
+  <si>
+    <t>Joel: Bot will ignore chat message posing as a sub alert</t>
+  </si>
+  <si>
+    <t>Joel: User inputs !gamble command incorrectly</t>
+  </si>
+  <si>
+    <t>Joel: User uses !gamble</t>
+  </si>
+  <si>
+    <t>Class:  gamble</t>
+  </si>
+  <si>
+    <t>Joel: Test 6</t>
+  </si>
+  <si>
+    <t>User types in "!gamble johnny" in chat</t>
+  </si>
+  <si>
+    <t>ot should say 'You did not enter either tails or heads loser...smh'</t>
+  </si>
+  <si>
+    <t>Joel: Test 7</t>
+  </si>
+  <si>
+    <t>User types in "!gamble tails"</t>
+  </si>
+  <si>
+    <t>Bot tells the user whether they won the bet or not.</t>
+  </si>
+  <si>
+    <t>Class:  onSubHandler</t>
+  </si>
+  <si>
+    <t>Joel: Test 8</t>
+  </si>
+  <si>
+    <t>Joel: Test 9</t>
+  </si>
+  <si>
+    <t>Wait for a subscription</t>
+  </si>
+  <si>
+    <t>Message will appear in the command window saying "/*/*/*/*/*Subscriber has been detected/*/*/*/*/*"</t>
+  </si>
+  <si>
+    <t>User types "/*/*/*/*/*Subscriber has been detected/*/*/*/*/*" to see if the bot will be tricked into thinking there's a new sub</t>
+  </si>
+  <si>
+    <t>No new sub will be detected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1197,7 +1256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView topLeftCell="J21" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
@@ -2153,7 +2212,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="T2:T33" xr:uid="{78B1D5D1-D291-4BF8-8527-AFE85CD03A19}">
+    <dataValidation type="list" allowBlank="1" sqref="T2:T33">
       <formula1>"Passed,Failed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2163,7 +2222,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2230,11 +2289,11 @@
       </c>
       <c r="C9" s="20">
         <f>C7-C11</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="31">
         <f>C9/C7</f>
-        <v>0.23076923076923078</v>
+        <v>0.19230769230769232</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -2250,11 +2309,11 @@
       </c>
       <c r="C11" s="20">
         <f>SUM(C12:C13)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" s="31">
         <f>C11/C7</f>
-        <v>0.76923076923076927</v>
+        <v>0.80769230769230771</v>
       </c>
       <c r="E11" s="29"/>
     </row>
@@ -2268,7 +2327,7 @@
       </c>
       <c r="D12" s="31">
         <f>C12/C11</f>
-        <v>0.95</v>
+        <v>0.90476190476190477</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>51</v>
@@ -2280,11 +2339,11 @@
       </c>
       <c r="C13" s="36">
         <f>COUNTIF('Test Case Tracker'!G:G,B13)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="37">
         <f>C13/C11</f>
-        <v>0.05</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="E13" s="38" t="s">
         <v>52</v>
@@ -2309,16 +2368,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
@@ -2369,13 +2428,13 @@
     </row>
     <row r="2" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="D2" s="18">
         <v>1</v>
@@ -2398,7 +2457,7 @@
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="15"/>
@@ -2421,15 +2480,15 @@
       <c r="J3" s="6"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:20" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" s="43" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="D4" s="18">
         <v>1</v>
@@ -2461,7 +2520,7 @@
     </row>
     <row r="5" spans="1:20" s="28" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="15"/>
@@ -2469,7 +2528,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>75</v>
@@ -2487,13 +2546,13 @@
     </row>
     <row r="6" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D6" s="19">
         <v>1</v>
@@ -2517,7 +2576,7 @@
     </row>
     <row r="7" spans="1:20" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -2543,13 +2602,13 @@
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="D8" s="19">
         <v>1</v>
@@ -2572,132 +2631,118 @@
     </row>
     <row r="9" spans="1:20" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="B9" s="3">
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="D9" s="19">
         <v>1</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>24</v>
+        <v>117</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="H9" s="5"/>
       <c r="I9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="J9" s="6"/>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="B10" s="3">
         <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="D10" s="19">
         <v>1</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="H10" s="5"/>
       <c r="I10" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>4</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="J10" s="6"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="B11" s="3">
         <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>29</v>
+        <v>122</v>
       </c>
       <c r="D11" s="19">
         <v>1</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="H11" s="5"/>
       <c r="I11" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>37</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="J11" s="9"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="B12" s="3">
         <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="D12" s="19">
         <v>1</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="5"/>
       <c r="I12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>37</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="J12" s="9"/>
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3150,7 +3195,7 @@
     <row r="28" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="G2:G27" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G27">
       <formula1>"Passed,Failed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3161,7 +3206,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3216,7 +3261,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added my screenshots for Asg15
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
+++ b/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\WebstormProjects\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="163">
   <si>
     <t>Expectations</t>
   </si>
@@ -652,6 +652,24 @@
   </si>
   <si>
     <t>Ad92jd2@!</t>
+  </si>
+  <si>
+    <t>Bot connected with no problems</t>
+  </si>
+  <si>
+    <t>User CowboyCat44 was slapped in chat</t>
+  </si>
+  <si>
+    <t>User could not be slapped because no user of that name exists</t>
+  </si>
+  <si>
+    <t>Bot connected</t>
+  </si>
+  <si>
+    <t>Return null status because user CowboyCat44 has no badges</t>
+  </si>
+  <si>
+    <t>I slapped the user 'cowboycat44'</t>
   </si>
 </sst>
 </file>
@@ -4426,8 +4444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5098,7 +5116,9 @@
       <c r="G18" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="22"/>
+      <c r="H18" s="22" t="s">
+        <v>157</v>
+      </c>
       <c r="I18" s="23" t="s">
         <v>17</v>
       </c>
@@ -5134,7 +5154,9 @@
       <c r="G19" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="22"/>
+      <c r="H19" s="22" t="s">
+        <v>158</v>
+      </c>
       <c r="I19" s="23" t="s">
         <v>17</v>
       </c>
@@ -5170,7 +5192,9 @@
       <c r="G20" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="22"/>
+      <c r="H20" s="22" t="s">
+        <v>162</v>
+      </c>
       <c r="I20" s="23" t="s">
         <v>17</v>
       </c>
@@ -5206,7 +5230,9 @@
       <c r="G21" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="22" t="s">
+        <v>159</v>
+      </c>
       <c r="I21" s="23" t="s">
         <v>17</v>
       </c>
@@ -5246,7 +5272,9 @@
       <c r="G22" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="22"/>
+      <c r="H22" s="22" t="s">
+        <v>160</v>
+      </c>
       <c r="I22" s="23" t="s">
         <v>17</v>
       </c>
@@ -5282,7 +5310,9 @@
       <c r="G23" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="22"/>
+      <c r="H23" s="22" t="s">
+        <v>161</v>
+      </c>
       <c r="I23" s="23" t="s">
         <v>17</v>
       </c>
@@ -5323,7 +5353,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>54</v>
+        <v>158</v>
       </c>
       <c r="I24" s="23" t="s">
         <v>17</v>
@@ -5365,7 +5395,7 @@
         <v>16</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>54</v>
+        <v>162</v>
       </c>
       <c r="I25" s="23" t="s">
         <v>17</v>
@@ -5407,7 +5437,7 @@
         <v>16</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>54</v>
+        <v>159</v>
       </c>
       <c r="I26" s="23" t="s">
         <v>17</v>
@@ -5449,7 +5479,7 @@
         <v>16</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="I27" s="23" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Update test tracker and moderator checks
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
+++ b/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NinoPinto\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99282373-C46A-4DB3-B6B3-2DB2A3115CE7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE81A05-FFBD-4493-BD2B-74024EBF2730}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,11 +19,12 @@
     <sheet name="Test Creation Assigments" sheetId="4" r:id="rId4"/>
     <sheet name="Test Data" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179021" calcMode="manual"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -189,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="217">
   <si>
     <t>Expectations</t>
   </si>
@@ -738,13 +739,115 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Class:  exitListen</t>
+  </si>
+  <si>
+    <t>Michael: Broadcaster tries to exit bot in terminal</t>
+  </si>
+  <si>
+    <t>Broadcaster types 'exit' in terminal</t>
+  </si>
+  <si>
+    <t>Bot should immediately stop execution and terminate process</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Bot exited successfully</t>
+  </si>
+  <si>
+    <t>Michael: Broadcaster tries to exit bot in terminal but makes a typo</t>
+  </si>
+  <si>
+    <t>Broadcaster types  'bananaphone' in terminal</t>
+  </si>
+  <si>
+    <t>Bot should ignore input and do nothing</t>
+  </si>
+  <si>
+    <t>Nothing happens</t>
+  </si>
+  <si>
+    <t>Michael: Moderator uses !allowrequests command</t>
+  </si>
+  <si>
+    <t>Moderator types !allowrequests for first time</t>
+  </si>
+  <si>
+    <t>Bot creates a new youtube playlist and allows requestsong command to add songs</t>
+  </si>
+  <si>
+    <t>Bot creates playlist and posts ID of playlist in terminal</t>
+  </si>
+  <si>
+    <t>Michael: User (non-mod) uses !allowrequests</t>
+  </si>
+  <si>
+    <t>User types !allowrequests in chat</t>
+  </si>
+  <si>
+    <t>Bot should ignore command and give chat error message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does not activate requestsong and posts </t>
+  </si>
+  <si>
+    <t>Class: requestsong</t>
+  </si>
+  <si>
+    <t>Class: allowrequests</t>
+  </si>
+  <si>
+    <t>Michael: User types !requestsong with proper format</t>
+  </si>
+  <si>
+    <t>!requestsong used with proper YT url</t>
+  </si>
+  <si>
+    <t>Bot should add song to playlist (after !allowrequests is used) and return video info to terminal</t>
+  </si>
+  <si>
+    <t>Bot adds song to playlist generated in YT account of broadcaster</t>
+  </si>
+  <si>
+    <t>Michael: User types !requestsong with just video ID</t>
+  </si>
+  <si>
+    <t>!requestsong used with just YT video ID</t>
+  </si>
+  <si>
+    <t>Michael: User types !request song with invalid URL</t>
+  </si>
+  <si>
+    <t>!requestsong used with any URL but YT or non-URL string</t>
+  </si>
+  <si>
+    <t>Bot should ignore and give error message</t>
+  </si>
+  <si>
+    <t>Class: blockrequests</t>
+  </si>
+  <si>
+    <t>Michael: Moderator uses !blockrequests</t>
+  </si>
+  <si>
+    <t>Moderator types !blockrequests in chat</t>
+  </si>
+  <si>
+    <t>Bot should turn off song requests and no longer accept !requestsong command</t>
+  </si>
+  <si>
+    <t>Request song no longer works</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -773,6 +876,12 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1198,7 +1307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1419,14 +1528,27 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4421,8 +4543,8 @@
         <v>103</v>
       </c>
       <c r="C5" s="37">
-        <f>COUNT('Test Case Tracker'!B1:B46)</f>
-        <v>27</v>
+        <f>COUNT('Test Case Tracker'!B1:B49)</f>
+        <v>30</v>
       </c>
       <c r="D5" s="38"/>
       <c r="E5" s="3"/>
@@ -4439,9 +4561,9 @@
       <c r="B7" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="105">
-        <f>COUNTA('Test Case Tracker'!D1:D46)-1</f>
-        <v>42</v>
+      <c r="C7" s="104">
+        <f>COUNTA('Test Case Tracker'!D1:D49)-1</f>
+        <v>45</v>
       </c>
       <c r="D7" s="42"/>
       <c r="E7" s="43"/>
@@ -4460,11 +4582,11 @@
       </c>
       <c r="C9" s="48">
         <f>C7-C11</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D9" s="49">
         <f>C9/C7</f>
-        <v>0.26190476190476192</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="E9" s="46"/>
     </row>
@@ -4482,11 +4604,11 @@
       </c>
       <c r="C11" s="48">
         <f>SUM(C12:C13)</f>
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D11" s="49">
         <f>C11/C7</f>
-        <v>0.73809523809523814</v>
+        <v>0.84444444444444444</v>
       </c>
       <c r="E11" s="46"/>
     </row>
@@ -4496,12 +4618,12 @@
         <v>16</v>
       </c>
       <c r="C12" s="48">
-        <f>COUNTIF('Test Case Tracker'!G1:G37,B12)</f>
-        <v>27</v>
+        <f>COUNTIF('Test Case Tracker'!G1:G40,B12)</f>
+        <v>34</v>
       </c>
       <c r="D12" s="49">
         <f>C12/C11</f>
-        <v>0.87096774193548387</v>
+        <v>0.89473684210526316</v>
       </c>
       <c r="E12" s="52" t="s">
         <v>107</v>
@@ -4513,12 +4635,12 @@
         <v>42</v>
       </c>
       <c r="C13" s="54">
-        <f>COUNTIF('Test Case Tracker'!G1:G37,B13)</f>
+        <f>COUNTIF('Test Case Tracker'!G1:G40,B13)</f>
         <v>4</v>
       </c>
       <c r="D13" s="55">
         <f>C13/C11</f>
-        <v>0.12903225806451613</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="E13" s="56" t="s">
         <v>108</v>
@@ -4558,10 +4680,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV44"/>
+  <dimension ref="A1:IV47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5032,29 +5154,35 @@
     </row>
     <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>50</v>
+        <v>183</v>
       </c>
       <c r="B13" s="17">
         <v>9</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>61</v>
+        <v>184</v>
       </c>
       <c r="D13" s="19">
         <v>1</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>52</v>
+        <v>185</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="28"/>
+        <v>186</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="H13" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
+        <v>188</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>170</v>
+      </c>
       <c r="K13" s="65"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -5067,30 +5195,34 @@
       <c r="T13" s="3"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>63</v>
-      </c>
+      <c r="A14" s="16"/>
       <c r="B14" s="17">
         <v>10</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>64</v>
+        <v>189</v>
       </c>
       <c r="D14" s="19">
         <v>1</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>52</v>
+        <v>190</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="28"/>
+        <v>191</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="H14" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="29"/>
+        <v>192</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>170</v>
+      </c>
       <c r="K14" s="65"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -5102,31 +5234,37 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>63</v>
+        <v>202</v>
       </c>
       <c r="B15" s="17">
         <v>11</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
       <c r="D15" s="19">
         <v>1</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>52</v>
+        <v>194</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="28"/>
+        <v>195</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="H15" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="29"/>
+        <v>196</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>170</v>
+      </c>
       <c r="K15" s="65"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -5139,30 +5277,34 @@
       <c r="T15" s="3"/>
     </row>
     <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>63</v>
-      </c>
+      <c r="A16" s="16"/>
       <c r="B16" s="17">
         <v>12</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>66</v>
+        <v>197</v>
       </c>
       <c r="D16" s="19">
         <v>1</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>52</v>
+        <v>198</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="28"/>
+        <v>199</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>16</v>
+      </c>
       <c r="H16" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="29"/>
+        <v>200</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="J16" s="29" t="s">
+        <v>170</v>
+      </c>
       <c r="K16" s="65"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -5174,31 +5316,37 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
-        <v>63</v>
+    <row r="17" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="110" t="s">
+        <v>212</v>
       </c>
       <c r="B17" s="17">
         <v>13</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>67</v>
+      <c r="C17" s="105" t="s">
+        <v>213</v>
       </c>
       <c r="D17" s="19">
         <v>1</v>
       </c>
-      <c r="E17" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
+      <c r="E17" s="106" t="s">
+        <v>214</v>
+      </c>
+      <c r="F17" s="106" t="s">
+        <v>215</v>
+      </c>
+      <c r="G17" s="107" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="106" t="s">
+        <v>216</v>
+      </c>
+      <c r="I17" s="108" t="s">
+        <v>187</v>
+      </c>
+      <c r="J17" s="109" t="s">
+        <v>170</v>
+      </c>
       <c r="K17" s="65"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -5209,37 +5357,273 @@
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
-    </row>
-    <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U17" s="91"/>
+      <c r="V17" s="91"/>
+      <c r="W17" s="91"/>
+      <c r="X17" s="91"/>
+      <c r="Y17" s="91"/>
+      <c r="Z17" s="91"/>
+      <c r="AA17" s="91"/>
+      <c r="AB17" s="91"/>
+      <c r="AC17" s="91"/>
+      <c r="AD17" s="91"/>
+      <c r="AE17" s="91"/>
+      <c r="AF17" s="91"/>
+      <c r="AG17" s="91"/>
+      <c r="AH17" s="91"/>
+      <c r="AI17" s="91"/>
+      <c r="AJ17" s="91"/>
+      <c r="AK17" s="91"/>
+      <c r="AL17" s="91"/>
+      <c r="AM17" s="91"/>
+      <c r="AN17" s="91"/>
+      <c r="AO17" s="91"/>
+      <c r="AP17" s="91"/>
+      <c r="AQ17" s="91"/>
+      <c r="AR17" s="91"/>
+      <c r="AS17" s="91"/>
+      <c r="AT17" s="91"/>
+      <c r="AU17" s="91"/>
+      <c r="AV17" s="91"/>
+      <c r="AW17" s="91"/>
+      <c r="AX17" s="91"/>
+      <c r="AY17" s="91"/>
+      <c r="AZ17" s="91"/>
+      <c r="BA17" s="91"/>
+      <c r="BB17" s="91"/>
+      <c r="BC17" s="91"/>
+      <c r="BD17" s="91"/>
+      <c r="BE17" s="91"/>
+      <c r="BF17" s="91"/>
+      <c r="BG17" s="91"/>
+      <c r="BH17" s="91"/>
+      <c r="BI17" s="91"/>
+      <c r="BJ17" s="91"/>
+      <c r="BK17" s="91"/>
+      <c r="BL17" s="91"/>
+      <c r="BM17" s="91"/>
+      <c r="BN17" s="91"/>
+      <c r="BO17" s="91"/>
+      <c r="BP17" s="91"/>
+      <c r="BQ17" s="91"/>
+      <c r="BR17" s="91"/>
+      <c r="BS17" s="91"/>
+      <c r="BT17" s="91"/>
+      <c r="BU17" s="91"/>
+      <c r="BV17" s="91"/>
+      <c r="BW17" s="91"/>
+      <c r="BX17" s="91"/>
+      <c r="BY17" s="91"/>
+      <c r="BZ17" s="91"/>
+      <c r="CA17" s="91"/>
+      <c r="CB17" s="91"/>
+      <c r="CC17" s="91"/>
+      <c r="CD17" s="91"/>
+      <c r="CE17" s="91"/>
+      <c r="CF17" s="91"/>
+      <c r="CG17" s="91"/>
+      <c r="CH17" s="91"/>
+      <c r="CI17" s="91"/>
+      <c r="CJ17" s="91"/>
+      <c r="CK17" s="91"/>
+      <c r="CL17" s="91"/>
+      <c r="CM17" s="91"/>
+      <c r="CN17" s="91"/>
+      <c r="CO17" s="91"/>
+      <c r="CP17" s="91"/>
+      <c r="CQ17" s="91"/>
+      <c r="CR17" s="91"/>
+      <c r="CS17" s="91"/>
+      <c r="CT17" s="91"/>
+      <c r="CU17" s="91"/>
+      <c r="CV17" s="91"/>
+      <c r="CW17" s="91"/>
+      <c r="CX17" s="91"/>
+      <c r="CY17" s="91"/>
+      <c r="CZ17" s="91"/>
+      <c r="DA17" s="91"/>
+      <c r="DB17" s="91"/>
+      <c r="DC17" s="91"/>
+      <c r="DD17" s="91"/>
+      <c r="DE17" s="91"/>
+      <c r="DF17" s="91"/>
+      <c r="DG17" s="91"/>
+      <c r="DH17" s="91"/>
+      <c r="DI17" s="91"/>
+      <c r="DJ17" s="91"/>
+      <c r="DK17" s="91"/>
+      <c r="DL17" s="91"/>
+      <c r="DM17" s="91"/>
+      <c r="DN17" s="91"/>
+      <c r="DO17" s="91"/>
+      <c r="DP17" s="91"/>
+      <c r="DQ17" s="91"/>
+      <c r="DR17" s="91"/>
+      <c r="DS17" s="91"/>
+      <c r="DT17" s="91"/>
+      <c r="DU17" s="91"/>
+      <c r="DV17" s="91"/>
+      <c r="DW17" s="91"/>
+      <c r="DX17" s="91"/>
+      <c r="DY17" s="91"/>
+      <c r="DZ17" s="91"/>
+      <c r="EA17" s="91"/>
+      <c r="EB17" s="91"/>
+      <c r="EC17" s="91"/>
+      <c r="ED17" s="91"/>
+      <c r="EE17" s="91"/>
+      <c r="EF17" s="91"/>
+      <c r="EG17" s="91"/>
+      <c r="EH17" s="91"/>
+      <c r="EI17" s="91"/>
+      <c r="EJ17" s="91"/>
+      <c r="EK17" s="91"/>
+      <c r="EL17" s="91"/>
+      <c r="EM17" s="91"/>
+      <c r="EN17" s="91"/>
+      <c r="EO17" s="91"/>
+      <c r="EP17" s="91"/>
+      <c r="EQ17" s="91"/>
+      <c r="ER17" s="91"/>
+      <c r="ES17" s="91"/>
+      <c r="ET17" s="91"/>
+      <c r="EU17" s="91"/>
+      <c r="EV17" s="91"/>
+      <c r="EW17" s="91"/>
+      <c r="EX17" s="91"/>
+      <c r="EY17" s="91"/>
+      <c r="EZ17" s="91"/>
+      <c r="FA17" s="91"/>
+      <c r="FB17" s="91"/>
+      <c r="FC17" s="91"/>
+      <c r="FD17" s="91"/>
+      <c r="FE17" s="91"/>
+      <c r="FF17" s="91"/>
+      <c r="FG17" s="91"/>
+      <c r="FH17" s="91"/>
+      <c r="FI17" s="91"/>
+      <c r="FJ17" s="91"/>
+      <c r="FK17" s="91"/>
+      <c r="FL17" s="91"/>
+      <c r="FM17" s="91"/>
+      <c r="FN17" s="91"/>
+      <c r="FO17" s="91"/>
+      <c r="FP17" s="91"/>
+      <c r="FQ17" s="91"/>
+      <c r="FR17" s="91"/>
+      <c r="FS17" s="91"/>
+      <c r="FT17" s="91"/>
+      <c r="FU17" s="91"/>
+      <c r="FV17" s="91"/>
+      <c r="FW17" s="91"/>
+      <c r="FX17" s="91"/>
+      <c r="FY17" s="91"/>
+      <c r="FZ17" s="91"/>
+      <c r="GA17" s="91"/>
+      <c r="GB17" s="91"/>
+      <c r="GC17" s="91"/>
+      <c r="GD17" s="91"/>
+      <c r="GE17" s="91"/>
+      <c r="GF17" s="91"/>
+      <c r="GG17" s="91"/>
+      <c r="GH17" s="91"/>
+      <c r="GI17" s="91"/>
+      <c r="GJ17" s="91"/>
+      <c r="GK17" s="91"/>
+      <c r="GL17" s="91"/>
+      <c r="GM17" s="91"/>
+      <c r="GN17" s="91"/>
+      <c r="GO17" s="91"/>
+      <c r="GP17" s="91"/>
+      <c r="GQ17" s="91"/>
+      <c r="GR17" s="91"/>
+      <c r="GS17" s="91"/>
+      <c r="GT17" s="91"/>
+      <c r="GU17" s="91"/>
+      <c r="GV17" s="91"/>
+      <c r="GW17" s="91"/>
+      <c r="GX17" s="91"/>
+      <c r="GY17" s="91"/>
+      <c r="GZ17" s="91"/>
+      <c r="HA17" s="91"/>
+      <c r="HB17" s="91"/>
+      <c r="HC17" s="91"/>
+      <c r="HD17" s="91"/>
+      <c r="HE17" s="91"/>
+      <c r="HF17" s="91"/>
+      <c r="HG17" s="91"/>
+      <c r="HH17" s="91"/>
+      <c r="HI17" s="91"/>
+      <c r="HJ17" s="91"/>
+      <c r="HK17" s="91"/>
+      <c r="HL17" s="91"/>
+      <c r="HM17" s="91"/>
+      <c r="HN17" s="91"/>
+      <c r="HO17" s="91"/>
+      <c r="HP17" s="91"/>
+      <c r="HQ17" s="91"/>
+      <c r="HR17" s="91"/>
+      <c r="HS17" s="91"/>
+      <c r="HT17" s="91"/>
+      <c r="HU17" s="91"/>
+      <c r="HV17" s="91"/>
+      <c r="HW17" s="91"/>
+      <c r="HX17" s="91"/>
+      <c r="HY17" s="91"/>
+      <c r="HZ17" s="91"/>
+      <c r="IA17" s="91"/>
+      <c r="IB17" s="91"/>
+      <c r="IC17" s="91"/>
+      <c r="ID17" s="91"/>
+      <c r="IE17" s="91"/>
+      <c r="IF17" s="91"/>
+      <c r="IG17" s="91"/>
+      <c r="IH17" s="91"/>
+      <c r="II17" s="91"/>
+      <c r="IJ17" s="91"/>
+      <c r="IK17" s="91"/>
+      <c r="IL17" s="91"/>
+      <c r="IM17" s="91"/>
+      <c r="IN17" s="91"/>
+      <c r="IO17" s="91"/>
+      <c r="IP17" s="91"/>
+      <c r="IQ17" s="91"/>
+      <c r="IR17" s="91"/>
+      <c r="IS17" s="91"/>
+      <c r="IT17" s="91"/>
+      <c r="IU17" s="91"/>
+      <c r="IV17" s="91"/>
+    </row>
+    <row r="18" spans="1:256" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>68</v>
+        <v>201</v>
       </c>
       <c r="B18" s="17">
         <v>14</v>
       </c>
-      <c r="C18" s="26" t="s">
-        <v>13</v>
+      <c r="C18" s="105" t="s">
+        <v>203</v>
       </c>
       <c r="D18" s="19">
         <v>1</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="21" t="s">
+      <c r="E18" s="106" t="s">
+        <v>204</v>
+      </c>
+      <c r="F18" s="106" t="s">
+        <v>205</v>
+      </c>
+      <c r="G18" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>35</v>
+      <c r="H18" s="106" t="s">
+        <v>206</v>
+      </c>
+      <c r="I18" s="108" t="s">
+        <v>187</v>
+      </c>
+      <c r="J18" s="109" t="s">
+        <v>170</v>
       </c>
       <c r="K18" s="65"/>
       <c r="L18" s="3"/>
@@ -5251,33 +5635,266 @@
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-    </row>
-    <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
+      <c r="U18" s="91"/>
+      <c r="V18" s="91"/>
+      <c r="W18" s="91"/>
+      <c r="X18" s="91"/>
+      <c r="Y18" s="91"/>
+      <c r="Z18" s="91"/>
+      <c r="AA18" s="91"/>
+      <c r="AB18" s="91"/>
+      <c r="AC18" s="91"/>
+      <c r="AD18" s="91"/>
+      <c r="AE18" s="91"/>
+      <c r="AF18" s="91"/>
+      <c r="AG18" s="91"/>
+      <c r="AH18" s="91"/>
+      <c r="AI18" s="91"/>
+      <c r="AJ18" s="91"/>
+      <c r="AK18" s="91"/>
+      <c r="AL18" s="91"/>
+      <c r="AM18" s="91"/>
+      <c r="AN18" s="91"/>
+      <c r="AO18" s="91"/>
+      <c r="AP18" s="91"/>
+      <c r="AQ18" s="91"/>
+      <c r="AR18" s="91"/>
+      <c r="AS18" s="91"/>
+      <c r="AT18" s="91"/>
+      <c r="AU18" s="91"/>
+      <c r="AV18" s="91"/>
+      <c r="AW18" s="91"/>
+      <c r="AX18" s="91"/>
+      <c r="AY18" s="91"/>
+      <c r="AZ18" s="91"/>
+      <c r="BA18" s="91"/>
+      <c r="BB18" s="91"/>
+      <c r="BC18" s="91"/>
+      <c r="BD18" s="91"/>
+      <c r="BE18" s="91"/>
+      <c r="BF18" s="91"/>
+      <c r="BG18" s="91"/>
+      <c r="BH18" s="91"/>
+      <c r="BI18" s="91"/>
+      <c r="BJ18" s="91"/>
+      <c r="BK18" s="91"/>
+      <c r="BL18" s="91"/>
+      <c r="BM18" s="91"/>
+      <c r="BN18" s="91"/>
+      <c r="BO18" s="91"/>
+      <c r="BP18" s="91"/>
+      <c r="BQ18" s="91"/>
+      <c r="BR18" s="91"/>
+      <c r="BS18" s="91"/>
+      <c r="BT18" s="91"/>
+      <c r="BU18" s="91"/>
+      <c r="BV18" s="91"/>
+      <c r="BW18" s="91"/>
+      <c r="BX18" s="91"/>
+      <c r="BY18" s="91"/>
+      <c r="BZ18" s="91"/>
+      <c r="CA18" s="91"/>
+      <c r="CB18" s="91"/>
+      <c r="CC18" s="91"/>
+      <c r="CD18" s="91"/>
+      <c r="CE18" s="91"/>
+      <c r="CF18" s="91"/>
+      <c r="CG18" s="91"/>
+      <c r="CH18" s="91"/>
+      <c r="CI18" s="91"/>
+      <c r="CJ18" s="91"/>
+      <c r="CK18" s="91"/>
+      <c r="CL18" s="91"/>
+      <c r="CM18" s="91"/>
+      <c r="CN18" s="91"/>
+      <c r="CO18" s="91"/>
+      <c r="CP18" s="91"/>
+      <c r="CQ18" s="91"/>
+      <c r="CR18" s="91"/>
+      <c r="CS18" s="91"/>
+      <c r="CT18" s="91"/>
+      <c r="CU18" s="91"/>
+      <c r="CV18" s="91"/>
+      <c r="CW18" s="91"/>
+      <c r="CX18" s="91"/>
+      <c r="CY18" s="91"/>
+      <c r="CZ18" s="91"/>
+      <c r="DA18" s="91"/>
+      <c r="DB18" s="91"/>
+      <c r="DC18" s="91"/>
+      <c r="DD18" s="91"/>
+      <c r="DE18" s="91"/>
+      <c r="DF18" s="91"/>
+      <c r="DG18" s="91"/>
+      <c r="DH18" s="91"/>
+      <c r="DI18" s="91"/>
+      <c r="DJ18" s="91"/>
+      <c r="DK18" s="91"/>
+      <c r="DL18" s="91"/>
+      <c r="DM18" s="91"/>
+      <c r="DN18" s="91"/>
+      <c r="DO18" s="91"/>
+      <c r="DP18" s="91"/>
+      <c r="DQ18" s="91"/>
+      <c r="DR18" s="91"/>
+      <c r="DS18" s="91"/>
+      <c r="DT18" s="91"/>
+      <c r="DU18" s="91"/>
+      <c r="DV18" s="91"/>
+      <c r="DW18" s="91"/>
+      <c r="DX18" s="91"/>
+      <c r="DY18" s="91"/>
+      <c r="DZ18" s="91"/>
+      <c r="EA18" s="91"/>
+      <c r="EB18" s="91"/>
+      <c r="EC18" s="91"/>
+      <c r="ED18" s="91"/>
+      <c r="EE18" s="91"/>
+      <c r="EF18" s="91"/>
+      <c r="EG18" s="91"/>
+      <c r="EH18" s="91"/>
+      <c r="EI18" s="91"/>
+      <c r="EJ18" s="91"/>
+      <c r="EK18" s="91"/>
+      <c r="EL18" s="91"/>
+      <c r="EM18" s="91"/>
+      <c r="EN18" s="91"/>
+      <c r="EO18" s="91"/>
+      <c r="EP18" s="91"/>
+      <c r="EQ18" s="91"/>
+      <c r="ER18" s="91"/>
+      <c r="ES18" s="91"/>
+      <c r="ET18" s="91"/>
+      <c r="EU18" s="91"/>
+      <c r="EV18" s="91"/>
+      <c r="EW18" s="91"/>
+      <c r="EX18" s="91"/>
+      <c r="EY18" s="91"/>
+      <c r="EZ18" s="91"/>
+      <c r="FA18" s="91"/>
+      <c r="FB18" s="91"/>
+      <c r="FC18" s="91"/>
+      <c r="FD18" s="91"/>
+      <c r="FE18" s="91"/>
+      <c r="FF18" s="91"/>
+      <c r="FG18" s="91"/>
+      <c r="FH18" s="91"/>
+      <c r="FI18" s="91"/>
+      <c r="FJ18" s="91"/>
+      <c r="FK18" s="91"/>
+      <c r="FL18" s="91"/>
+      <c r="FM18" s="91"/>
+      <c r="FN18" s="91"/>
+      <c r="FO18" s="91"/>
+      <c r="FP18" s="91"/>
+      <c r="FQ18" s="91"/>
+      <c r="FR18" s="91"/>
+      <c r="FS18" s="91"/>
+      <c r="FT18" s="91"/>
+      <c r="FU18" s="91"/>
+      <c r="FV18" s="91"/>
+      <c r="FW18" s="91"/>
+      <c r="FX18" s="91"/>
+      <c r="FY18" s="91"/>
+      <c r="FZ18" s="91"/>
+      <c r="GA18" s="91"/>
+      <c r="GB18" s="91"/>
+      <c r="GC18" s="91"/>
+      <c r="GD18" s="91"/>
+      <c r="GE18" s="91"/>
+      <c r="GF18" s="91"/>
+      <c r="GG18" s="91"/>
+      <c r="GH18" s="91"/>
+      <c r="GI18" s="91"/>
+      <c r="GJ18" s="91"/>
+      <c r="GK18" s="91"/>
+      <c r="GL18" s="91"/>
+      <c r="GM18" s="91"/>
+      <c r="GN18" s="91"/>
+      <c r="GO18" s="91"/>
+      <c r="GP18" s="91"/>
+      <c r="GQ18" s="91"/>
+      <c r="GR18" s="91"/>
+      <c r="GS18" s="91"/>
+      <c r="GT18" s="91"/>
+      <c r="GU18" s="91"/>
+      <c r="GV18" s="91"/>
+      <c r="GW18" s="91"/>
+      <c r="GX18" s="91"/>
+      <c r="GY18" s="91"/>
+      <c r="GZ18" s="91"/>
+      <c r="HA18" s="91"/>
+      <c r="HB18" s="91"/>
+      <c r="HC18" s="91"/>
+      <c r="HD18" s="91"/>
+      <c r="HE18" s="91"/>
+      <c r="HF18" s="91"/>
+      <c r="HG18" s="91"/>
+      <c r="HH18" s="91"/>
+      <c r="HI18" s="91"/>
+      <c r="HJ18" s="91"/>
+      <c r="HK18" s="91"/>
+      <c r="HL18" s="91"/>
+      <c r="HM18" s="91"/>
+      <c r="HN18" s="91"/>
+      <c r="HO18" s="91"/>
+      <c r="HP18" s="91"/>
+      <c r="HQ18" s="91"/>
+      <c r="HR18" s="91"/>
+      <c r="HS18" s="91"/>
+      <c r="HT18" s="91"/>
+      <c r="HU18" s="91"/>
+      <c r="HV18" s="91"/>
+      <c r="HW18" s="91"/>
+      <c r="HX18" s="91"/>
+      <c r="HY18" s="91"/>
+      <c r="HZ18" s="91"/>
+      <c r="IA18" s="91"/>
+      <c r="IB18" s="91"/>
+      <c r="IC18" s="91"/>
+      <c r="ID18" s="91"/>
+      <c r="IE18" s="91"/>
+      <c r="IF18" s="91"/>
+      <c r="IG18" s="91"/>
+      <c r="IH18" s="91"/>
+      <c r="II18" s="91"/>
+      <c r="IJ18" s="91"/>
+      <c r="IK18" s="91"/>
+      <c r="IL18" s="91"/>
+      <c r="IM18" s="91"/>
+      <c r="IN18" s="91"/>
+      <c r="IO18" s="91"/>
+      <c r="IP18" s="91"/>
+      <c r="IQ18" s="91"/>
+      <c r="IR18" s="91"/>
+      <c r="IS18" s="91"/>
+      <c r="IT18" s="91"/>
+      <c r="IU18" s="91"/>
+      <c r="IV18" s="91"/>
+    </row>
+    <row r="19" spans="1:256" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B19" s="17">
+        <v>15</v>
+      </c>
+      <c r="C19" s="105" t="s">
+        <v>207</v>
+      </c>
       <c r="D19" s="19">
-        <v>2</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>35</v>
+        <v>1</v>
+      </c>
+      <c r="E19" s="106" t="s">
+        <v>208</v>
+      </c>
+      <c r="F19" s="106" t="s">
+        <v>205</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="108" t="s">
+        <v>187</v>
+      </c>
+      <c r="J19" s="109" t="s">
+        <v>170</v>
       </c>
       <c r="K19" s="65"/>
       <c r="L19" s="3"/>
@@ -5290,35 +5907,35 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
+    <row r="20" spans="1:256" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="91"/>
+      <c r="B20" s="17">
+        <v>16</v>
+      </c>
+      <c r="C20" s="105" t="s">
+        <v>209</v>
+      </c>
       <c r="D20" s="19">
-        <v>3</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="106" t="s">
+        <v>210</v>
+      </c>
+      <c r="F20" s="106" t="s">
+        <v>211</v>
+      </c>
+      <c r="G20" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="I20" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>35</v>
+      <c r="H20" s="20"/>
+      <c r="I20" s="108" t="s">
+        <v>187</v>
+      </c>
+      <c r="J20" s="109" t="s">
+        <v>170</v>
       </c>
       <c r="K20" s="65"/>
-      <c r="L20" s="33"/>
+      <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -5327,27 +5944,267 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
-    </row>
-    <row r="21" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U20" s="91"/>
+      <c r="V20" s="91"/>
+      <c r="W20" s="91"/>
+      <c r="X20" s="91"/>
+      <c r="Y20" s="91"/>
+      <c r="Z20" s="91"/>
+      <c r="AA20" s="91"/>
+      <c r="AB20" s="91"/>
+      <c r="AC20" s="91"/>
+      <c r="AD20" s="91"/>
+      <c r="AE20" s="91"/>
+      <c r="AF20" s="91"/>
+      <c r="AG20" s="91"/>
+      <c r="AH20" s="91"/>
+      <c r="AI20" s="91"/>
+      <c r="AJ20" s="91"/>
+      <c r="AK20" s="91"/>
+      <c r="AL20" s="91"/>
+      <c r="AM20" s="91"/>
+      <c r="AN20" s="91"/>
+      <c r="AO20" s="91"/>
+      <c r="AP20" s="91"/>
+      <c r="AQ20" s="91"/>
+      <c r="AR20" s="91"/>
+      <c r="AS20" s="91"/>
+      <c r="AT20" s="91"/>
+      <c r="AU20" s="91"/>
+      <c r="AV20" s="91"/>
+      <c r="AW20" s="91"/>
+      <c r="AX20" s="91"/>
+      <c r="AY20" s="91"/>
+      <c r="AZ20" s="91"/>
+      <c r="BA20" s="91"/>
+      <c r="BB20" s="91"/>
+      <c r="BC20" s="91"/>
+      <c r="BD20" s="91"/>
+      <c r="BE20" s="91"/>
+      <c r="BF20" s="91"/>
+      <c r="BG20" s="91"/>
+      <c r="BH20" s="91"/>
+      <c r="BI20" s="91"/>
+      <c r="BJ20" s="91"/>
+      <c r="BK20" s="91"/>
+      <c r="BL20" s="91"/>
+      <c r="BM20" s="91"/>
+      <c r="BN20" s="91"/>
+      <c r="BO20" s="91"/>
+      <c r="BP20" s="91"/>
+      <c r="BQ20" s="91"/>
+      <c r="BR20" s="91"/>
+      <c r="BS20" s="91"/>
+      <c r="BT20" s="91"/>
+      <c r="BU20" s="91"/>
+      <c r="BV20" s="91"/>
+      <c r="BW20" s="91"/>
+      <c r="BX20" s="91"/>
+      <c r="BY20" s="91"/>
+      <c r="BZ20" s="91"/>
+      <c r="CA20" s="91"/>
+      <c r="CB20" s="91"/>
+      <c r="CC20" s="91"/>
+      <c r="CD20" s="91"/>
+      <c r="CE20" s="91"/>
+      <c r="CF20" s="91"/>
+      <c r="CG20" s="91"/>
+      <c r="CH20" s="91"/>
+      <c r="CI20" s="91"/>
+      <c r="CJ20" s="91"/>
+      <c r="CK20" s="91"/>
+      <c r="CL20" s="91"/>
+      <c r="CM20" s="91"/>
+      <c r="CN20" s="91"/>
+      <c r="CO20" s="91"/>
+      <c r="CP20" s="91"/>
+      <c r="CQ20" s="91"/>
+      <c r="CR20" s="91"/>
+      <c r="CS20" s="91"/>
+      <c r="CT20" s="91"/>
+      <c r="CU20" s="91"/>
+      <c r="CV20" s="91"/>
+      <c r="CW20" s="91"/>
+      <c r="CX20" s="91"/>
+      <c r="CY20" s="91"/>
+      <c r="CZ20" s="91"/>
+      <c r="DA20" s="91"/>
+      <c r="DB20" s="91"/>
+      <c r="DC20" s="91"/>
+      <c r="DD20" s="91"/>
+      <c r="DE20" s="91"/>
+      <c r="DF20" s="91"/>
+      <c r="DG20" s="91"/>
+      <c r="DH20" s="91"/>
+      <c r="DI20" s="91"/>
+      <c r="DJ20" s="91"/>
+      <c r="DK20" s="91"/>
+      <c r="DL20" s="91"/>
+      <c r="DM20" s="91"/>
+      <c r="DN20" s="91"/>
+      <c r="DO20" s="91"/>
+      <c r="DP20" s="91"/>
+      <c r="DQ20" s="91"/>
+      <c r="DR20" s="91"/>
+      <c r="DS20" s="91"/>
+      <c r="DT20" s="91"/>
+      <c r="DU20" s="91"/>
+      <c r="DV20" s="91"/>
+      <c r="DW20" s="91"/>
+      <c r="DX20" s="91"/>
+      <c r="DY20" s="91"/>
+      <c r="DZ20" s="91"/>
+      <c r="EA20" s="91"/>
+      <c r="EB20" s="91"/>
+      <c r="EC20" s="91"/>
+      <c r="ED20" s="91"/>
+      <c r="EE20" s="91"/>
+      <c r="EF20" s="91"/>
+      <c r="EG20" s="91"/>
+      <c r="EH20" s="91"/>
+      <c r="EI20" s="91"/>
+      <c r="EJ20" s="91"/>
+      <c r="EK20" s="91"/>
+      <c r="EL20" s="91"/>
+      <c r="EM20" s="91"/>
+      <c r="EN20" s="91"/>
+      <c r="EO20" s="91"/>
+      <c r="EP20" s="91"/>
+      <c r="EQ20" s="91"/>
+      <c r="ER20" s="91"/>
+      <c r="ES20" s="91"/>
+      <c r="ET20" s="91"/>
+      <c r="EU20" s="91"/>
+      <c r="EV20" s="91"/>
+      <c r="EW20" s="91"/>
+      <c r="EX20" s="91"/>
+      <c r="EY20" s="91"/>
+      <c r="EZ20" s="91"/>
+      <c r="FA20" s="91"/>
+      <c r="FB20" s="91"/>
+      <c r="FC20" s="91"/>
+      <c r="FD20" s="91"/>
+      <c r="FE20" s="91"/>
+      <c r="FF20" s="91"/>
+      <c r="FG20" s="91"/>
+      <c r="FH20" s="91"/>
+      <c r="FI20" s="91"/>
+      <c r="FJ20" s="91"/>
+      <c r="FK20" s="91"/>
+      <c r="FL20" s="91"/>
+      <c r="FM20" s="91"/>
+      <c r="FN20" s="91"/>
+      <c r="FO20" s="91"/>
+      <c r="FP20" s="91"/>
+      <c r="FQ20" s="91"/>
+      <c r="FR20" s="91"/>
+      <c r="FS20" s="91"/>
+      <c r="FT20" s="91"/>
+      <c r="FU20" s="91"/>
+      <c r="FV20" s="91"/>
+      <c r="FW20" s="91"/>
+      <c r="FX20" s="91"/>
+      <c r="FY20" s="91"/>
+      <c r="FZ20" s="91"/>
+      <c r="GA20" s="91"/>
+      <c r="GB20" s="91"/>
+      <c r="GC20" s="91"/>
+      <c r="GD20" s="91"/>
+      <c r="GE20" s="91"/>
+      <c r="GF20" s="91"/>
+      <c r="GG20" s="91"/>
+      <c r="GH20" s="91"/>
+      <c r="GI20" s="91"/>
+      <c r="GJ20" s="91"/>
+      <c r="GK20" s="91"/>
+      <c r="GL20" s="91"/>
+      <c r="GM20" s="91"/>
+      <c r="GN20" s="91"/>
+      <c r="GO20" s="91"/>
+      <c r="GP20" s="91"/>
+      <c r="GQ20" s="91"/>
+      <c r="GR20" s="91"/>
+      <c r="GS20" s="91"/>
+      <c r="GT20" s="91"/>
+      <c r="GU20" s="91"/>
+      <c r="GV20" s="91"/>
+      <c r="GW20" s="91"/>
+      <c r="GX20" s="91"/>
+      <c r="GY20" s="91"/>
+      <c r="GZ20" s="91"/>
+      <c r="HA20" s="91"/>
+      <c r="HB20" s="91"/>
+      <c r="HC20" s="91"/>
+      <c r="HD20" s="91"/>
+      <c r="HE20" s="91"/>
+      <c r="HF20" s="91"/>
+      <c r="HG20" s="91"/>
+      <c r="HH20" s="91"/>
+      <c r="HI20" s="91"/>
+      <c r="HJ20" s="91"/>
+      <c r="HK20" s="91"/>
+      <c r="HL20" s="91"/>
+      <c r="HM20" s="91"/>
+      <c r="HN20" s="91"/>
+      <c r="HO20" s="91"/>
+      <c r="HP20" s="91"/>
+      <c r="HQ20" s="91"/>
+      <c r="HR20" s="91"/>
+      <c r="HS20" s="91"/>
+      <c r="HT20" s="91"/>
+      <c r="HU20" s="91"/>
+      <c r="HV20" s="91"/>
+      <c r="HW20" s="91"/>
+      <c r="HX20" s="91"/>
+      <c r="HY20" s="91"/>
+      <c r="HZ20" s="91"/>
+      <c r="IA20" s="91"/>
+      <c r="IB20" s="91"/>
+      <c r="IC20" s="91"/>
+      <c r="ID20" s="91"/>
+      <c r="IE20" s="91"/>
+      <c r="IF20" s="91"/>
+      <c r="IG20" s="91"/>
+      <c r="IH20" s="91"/>
+      <c r="II20" s="91"/>
+      <c r="IJ20" s="91"/>
+      <c r="IK20" s="91"/>
+      <c r="IL20" s="91"/>
+      <c r="IM20" s="91"/>
+      <c r="IN20" s="91"/>
+      <c r="IO20" s="91"/>
+      <c r="IP20" s="91"/>
+      <c r="IQ20" s="91"/>
+      <c r="IR20" s="91"/>
+      <c r="IS20" s="91"/>
+      <c r="IT20" s="91"/>
+      <c r="IU20" s="91"/>
+      <c r="IV20" s="91"/>
+    </row>
+    <row r="21" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
+      <c r="B21" s="17">
+        <v>17</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>13</v>
+      </c>
       <c r="D21" s="19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G21" s="21" t="s">
         <v>16</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I21" s="23" t="s">
         <v>17</v>
@@ -5356,7 +6213,7 @@
         <v>35</v>
       </c>
       <c r="K21" s="65"/>
-      <c r="L21" s="33"/>
+      <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
@@ -5366,30 +6223,26 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="17">
-        <v>15</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>28</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>16</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I22" s="23" t="s">
         <v>17</v>
@@ -5408,26 +6261,26 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:256" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
       <c r="D23" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I23" s="23" t="s">
         <v>17</v>
@@ -5436,7 +6289,7 @@
         <v>35</v>
       </c>
       <c r="K23" s="65"/>
-      <c r="L23" s="3"/>
+      <c r="L23" s="33"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -5446,39 +6299,35 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
     </row>
-    <row r="24" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:256" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="17">
-        <v>16</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>132</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G24" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="20" t="s">
-        <v>158</v>
+      <c r="H24" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="I24" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="29" t="s">
+      <c r="J24" s="24" t="s">
         <v>35</v>
       </c>
       <c r="K24" s="65"/>
-      <c r="L24" s="3"/>
+      <c r="L24" s="33"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -5488,35 +6337,35 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" s="17">
-        <v>17</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>133</v>
+        <v>18</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>28</v>
       </c>
       <c r="D25" s="19">
         <v>1</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G25" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="20" t="s">
-        <v>162</v>
+      <c r="H25" s="22" t="s">
+        <v>160</v>
       </c>
       <c r="I25" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="29" t="s">
+      <c r="J25" s="24" t="s">
         <v>35</v>
       </c>
       <c r="K25" s="65"/>
@@ -5530,35 +6379,31 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
     </row>
-    <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="17">
-        <v>18</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>71</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18"/>
       <c r="D26" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G26" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="20" t="s">
-        <v>159</v>
+      <c r="H26" s="22" t="s">
+        <v>161</v>
       </c>
       <c r="I26" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="24" t="s">
         <v>35</v>
       </c>
       <c r="K26" s="65"/>
@@ -5572,30 +6417,30 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:256" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B27" s="17">
         <v>19</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="D27" s="19">
         <v>1</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G27" s="21" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I27" s="23" t="s">
         <v>17</v>
@@ -5614,33 +6459,37 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B28" s="17">
         <v>20</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="D28" s="19">
         <v>1</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="G28" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="20"/>
+      <c r="H28" s="20" t="s">
+        <v>162</v>
+      </c>
       <c r="I28" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="J28" s="29"/>
+        <v>17</v>
+      </c>
+      <c r="J28" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="K28" s="65"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -5652,29 +6501,37 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="21"/>
+        <v>70</v>
+      </c>
+      <c r="B29" s="17">
+        <v>21</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>71</v>
+      </c>
       <c r="D29" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="G29" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="20"/>
+      <c r="H29" s="20" t="s">
+        <v>159</v>
+      </c>
       <c r="I29" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="J29" s="29"/>
+        <v>17</v>
+      </c>
+      <c r="J29" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="K29" s="65"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -5686,29 +6543,37 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
     </row>
-    <row r="30" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="21"/>
+        <v>74</v>
+      </c>
+      <c r="B30" s="17">
+        <v>22</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="D30" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="G30" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="20"/>
+      <c r="H30" s="20" t="s">
+        <v>161</v>
+      </c>
       <c r="I30" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="J30" s="29"/>
+        <v>17</v>
+      </c>
+      <c r="J30" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="K30" s="65"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -5720,15 +6585,15 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B31" s="17">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D31" s="19">
         <v>1</v>
@@ -5758,9 +6623,9 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
     </row>
-    <row r="32" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="21"/>
@@ -5768,10 +6633,10 @@
         <v>2</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G32" s="21" t="s">
         <v>16</v>
@@ -5794,7 +6659,7 @@
     </row>
     <row r="33" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="21"/>
@@ -5802,13 +6667,13 @@
         <v>3</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="23" t="s">
@@ -5828,22 +6693,22 @@
     </row>
     <row r="34" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B34" s="17">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>134</v>
+        <v>85</v>
       </c>
       <c r="D34" s="19">
         <v>1</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G34" s="21" t="s">
         <v>16</v>
@@ -5866,29 +6731,23 @@
     </row>
     <row r="35" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" s="17">
-        <v>23</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>135</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="21"/>
       <c r="D35" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G35" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>136</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H35" s="20"/>
       <c r="I35" s="23" t="s">
         <v>79</v>
       </c>
@@ -5906,25 +6765,21 @@
     </row>
     <row r="36" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="17">
-        <v>24</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>90</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="H36" s="20"/>
       <c r="I36" s="23" t="s">
@@ -5944,22 +6799,22 @@
     </row>
     <row r="37" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B37" s="17">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="D37" s="19">
         <v>1</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
       <c r="G37" s="21" t="s">
         <v>16</v>
@@ -5981,601 +6836,158 @@
       <c r="T37" s="3"/>
     </row>
     <row r="38" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="92" t="s">
-        <v>166</v>
-      </c>
-      <c r="B38" s="93">
-        <v>25</v>
-      </c>
-      <c r="C38" s="94" t="s">
-        <v>167</v>
-      </c>
-      <c r="D38" s="95">
+      <c r="A38" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="17">
+        <v>26</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="19">
         <v>1</v>
       </c>
-      <c r="E38" s="96" t="s">
-        <v>171</v>
-      </c>
-      <c r="F38" s="96" t="s">
-        <v>172</v>
-      </c>
-      <c r="G38" s="101"/>
-      <c r="H38" s="99"/>
-      <c r="I38" s="97" t="s">
-        <v>170</v>
-      </c>
-      <c r="J38" s="102"/>
-      <c r="K38" s="103"/>
-      <c r="L38" s="104"/>
-      <c r="M38" s="104"/>
-      <c r="N38" s="104"/>
-      <c r="O38" s="104"/>
-      <c r="P38" s="104"/>
-      <c r="Q38" s="104"/>
-      <c r="R38" s="104"/>
-      <c r="S38" s="104"/>
-      <c r="T38" s="104"/>
-      <c r="U38" s="91"/>
-      <c r="V38" s="91"/>
-      <c r="W38" s="91"/>
-      <c r="X38" s="91"/>
-      <c r="Y38" s="91"/>
-      <c r="Z38" s="91"/>
-      <c r="AA38" s="91"/>
-      <c r="AB38" s="91"/>
-      <c r="AC38" s="91"/>
-      <c r="AD38" s="91"/>
-      <c r="AE38" s="91"/>
-      <c r="AF38" s="91"/>
-      <c r="AG38" s="91"/>
-      <c r="AH38" s="91"/>
-      <c r="AI38" s="91"/>
-      <c r="AJ38" s="91"/>
-      <c r="AK38" s="91"/>
-      <c r="AL38" s="91"/>
-      <c r="AM38" s="91"/>
-      <c r="AN38" s="91"/>
-      <c r="AO38" s="91"/>
-      <c r="AP38" s="91"/>
-      <c r="AQ38" s="91"/>
-      <c r="AR38" s="91"/>
-      <c r="AS38" s="91"/>
-      <c r="AT38" s="91"/>
-      <c r="AU38" s="91"/>
-      <c r="AV38" s="91"/>
-      <c r="AW38" s="91"/>
-      <c r="AX38" s="91"/>
-      <c r="AY38" s="91"/>
-      <c r="AZ38" s="91"/>
-      <c r="BA38" s="91"/>
-      <c r="BB38" s="91"/>
-      <c r="BC38" s="91"/>
-      <c r="BD38" s="91"/>
-      <c r="BE38" s="91"/>
-      <c r="BF38" s="91"/>
-      <c r="BG38" s="91"/>
-      <c r="BH38" s="91"/>
-      <c r="BI38" s="91"/>
-      <c r="BJ38" s="91"/>
-      <c r="BK38" s="91"/>
-      <c r="BL38" s="91"/>
-      <c r="BM38" s="91"/>
-      <c r="BN38" s="91"/>
-      <c r="BO38" s="91"/>
-      <c r="BP38" s="91"/>
-      <c r="BQ38" s="91"/>
-      <c r="BR38" s="91"/>
-      <c r="BS38" s="91"/>
-      <c r="BT38" s="91"/>
-      <c r="BU38" s="91"/>
-      <c r="BV38" s="91"/>
-      <c r="BW38" s="91"/>
-      <c r="BX38" s="91"/>
-      <c r="BY38" s="91"/>
-      <c r="BZ38" s="91"/>
-      <c r="CA38" s="91"/>
-      <c r="CB38" s="91"/>
-      <c r="CC38" s="91"/>
-      <c r="CD38" s="91"/>
-      <c r="CE38" s="91"/>
-      <c r="CF38" s="91"/>
-      <c r="CG38" s="91"/>
-      <c r="CH38" s="91"/>
-      <c r="CI38" s="91"/>
-      <c r="CJ38" s="91"/>
-      <c r="CK38" s="91"/>
-      <c r="CL38" s="91"/>
-      <c r="CM38" s="91"/>
-      <c r="CN38" s="91"/>
-      <c r="CO38" s="91"/>
-      <c r="CP38" s="91"/>
-      <c r="CQ38" s="91"/>
-      <c r="CR38" s="91"/>
-      <c r="CS38" s="91"/>
-      <c r="CT38" s="91"/>
-      <c r="CU38" s="91"/>
-      <c r="CV38" s="91"/>
-      <c r="CW38" s="91"/>
-      <c r="CX38" s="91"/>
-      <c r="CY38" s="91"/>
-      <c r="CZ38" s="91"/>
-      <c r="DA38" s="91"/>
-      <c r="DB38" s="91"/>
-      <c r="DC38" s="91"/>
-      <c r="DD38" s="91"/>
-      <c r="DE38" s="91"/>
-      <c r="DF38" s="91"/>
-      <c r="DG38" s="91"/>
-      <c r="DH38" s="91"/>
-      <c r="DI38" s="91"/>
-      <c r="DJ38" s="91"/>
-      <c r="DK38" s="91"/>
-      <c r="DL38" s="91"/>
-      <c r="DM38" s="91"/>
-      <c r="DN38" s="91"/>
-      <c r="DO38" s="91"/>
-      <c r="DP38" s="91"/>
-      <c r="DQ38" s="91"/>
-      <c r="DR38" s="91"/>
-      <c r="DS38" s="91"/>
-      <c r="DT38" s="91"/>
-      <c r="DU38" s="91"/>
-      <c r="DV38" s="91"/>
-      <c r="DW38" s="91"/>
-      <c r="DX38" s="91"/>
-      <c r="DY38" s="91"/>
-      <c r="DZ38" s="91"/>
-      <c r="EA38" s="91"/>
-      <c r="EB38" s="91"/>
-      <c r="EC38" s="91"/>
-      <c r="ED38" s="91"/>
-      <c r="EE38" s="91"/>
-      <c r="EF38" s="91"/>
-      <c r="EG38" s="91"/>
-      <c r="EH38" s="91"/>
-      <c r="EI38" s="91"/>
-      <c r="EJ38" s="91"/>
-      <c r="EK38" s="91"/>
-      <c r="EL38" s="91"/>
-      <c r="EM38" s="91"/>
-      <c r="EN38" s="91"/>
-      <c r="EO38" s="91"/>
-      <c r="EP38" s="91"/>
-      <c r="EQ38" s="91"/>
-      <c r="ER38" s="91"/>
-      <c r="ES38" s="91"/>
-      <c r="ET38" s="91"/>
-      <c r="EU38" s="91"/>
-      <c r="EV38" s="91"/>
-      <c r="EW38" s="91"/>
-      <c r="EX38" s="91"/>
-      <c r="EY38" s="91"/>
-      <c r="EZ38" s="91"/>
-      <c r="FA38" s="91"/>
-      <c r="FB38" s="91"/>
-      <c r="FC38" s="91"/>
-      <c r="FD38" s="91"/>
-      <c r="FE38" s="91"/>
-      <c r="FF38" s="91"/>
-      <c r="FG38" s="91"/>
-      <c r="FH38" s="91"/>
-      <c r="FI38" s="91"/>
-      <c r="FJ38" s="91"/>
-      <c r="FK38" s="91"/>
-      <c r="FL38" s="91"/>
-      <c r="FM38" s="91"/>
-      <c r="FN38" s="91"/>
-      <c r="FO38" s="91"/>
-      <c r="FP38" s="91"/>
-      <c r="FQ38" s="91"/>
-      <c r="FR38" s="91"/>
-      <c r="FS38" s="91"/>
-      <c r="FT38" s="91"/>
-      <c r="FU38" s="91"/>
-      <c r="FV38" s="91"/>
-      <c r="FW38" s="91"/>
-      <c r="FX38" s="91"/>
-      <c r="FY38" s="91"/>
-      <c r="FZ38" s="91"/>
-      <c r="GA38" s="91"/>
-      <c r="GB38" s="91"/>
-      <c r="GC38" s="91"/>
-      <c r="GD38" s="91"/>
-      <c r="GE38" s="91"/>
-      <c r="GF38" s="91"/>
-      <c r="GG38" s="91"/>
-      <c r="GH38" s="91"/>
-      <c r="GI38" s="91"/>
-      <c r="GJ38" s="91"/>
-      <c r="GK38" s="91"/>
-      <c r="GL38" s="91"/>
-      <c r="GM38" s="91"/>
-      <c r="GN38" s="91"/>
-      <c r="GO38" s="91"/>
-      <c r="GP38" s="91"/>
-      <c r="GQ38" s="91"/>
-      <c r="GR38" s="91"/>
-      <c r="GS38" s="91"/>
-      <c r="GT38" s="91"/>
-      <c r="GU38" s="91"/>
-      <c r="GV38" s="91"/>
-      <c r="GW38" s="91"/>
-      <c r="GX38" s="91"/>
-      <c r="GY38" s="91"/>
-      <c r="GZ38" s="91"/>
-      <c r="HA38" s="91"/>
-      <c r="HB38" s="91"/>
-      <c r="HC38" s="91"/>
-      <c r="HD38" s="91"/>
-      <c r="HE38" s="91"/>
-      <c r="HF38" s="91"/>
-      <c r="HG38" s="91"/>
-      <c r="HH38" s="91"/>
-      <c r="HI38" s="91"/>
-      <c r="HJ38" s="91"/>
-      <c r="HK38" s="91"/>
-      <c r="HL38" s="91"/>
-      <c r="HM38" s="91"/>
-      <c r="HN38" s="91"/>
-      <c r="HO38" s="91"/>
-      <c r="HP38" s="91"/>
-      <c r="HQ38" s="91"/>
-      <c r="HR38" s="91"/>
-      <c r="HS38" s="91"/>
-      <c r="HT38" s="91"/>
-      <c r="HU38" s="91"/>
-      <c r="HV38" s="91"/>
-      <c r="HW38" s="91"/>
-      <c r="HX38" s="91"/>
-      <c r="HY38" s="91"/>
-      <c r="HZ38" s="91"/>
-      <c r="IA38" s="91"/>
-      <c r="IB38" s="91"/>
-      <c r="IC38" s="91"/>
-      <c r="ID38" s="91"/>
-      <c r="IE38" s="91"/>
-      <c r="IF38" s="91"/>
-      <c r="IG38" s="91"/>
-      <c r="IH38" s="91"/>
-      <c r="II38" s="91"/>
-      <c r="IJ38" s="91"/>
-      <c r="IK38" s="91"/>
-      <c r="IL38" s="91"/>
-      <c r="IM38" s="91"/>
-      <c r="IN38" s="91"/>
-      <c r="IO38" s="91"/>
-      <c r="IP38" s="91"/>
-      <c r="IQ38" s="91"/>
-      <c r="IR38" s="91"/>
-      <c r="IS38" s="91"/>
-      <c r="IT38" s="91"/>
-      <c r="IU38" s="91"/>
-      <c r="IV38" s="91"/>
-    </row>
-    <row r="39" spans="1:256" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="92" t="s">
-        <v>166</v>
-      </c>
-      <c r="B39" s="93"/>
-      <c r="C39" s="94" t="s">
-        <v>178</v>
-      </c>
-      <c r="D39" s="95">
-        <v>2</v>
-      </c>
-      <c r="E39" s="96" t="s">
-        <v>168</v>
-      </c>
-      <c r="F39" s="96" t="s">
-        <v>173</v>
-      </c>
-      <c r="I39" s="97" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="40" spans="1:256" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="92" t="s">
-        <v>166</v>
-      </c>
-      <c r="B40" s="93"/>
-      <c r="C40" s="94" t="s">
-        <v>174</v>
-      </c>
-      <c r="D40" s="98">
-        <v>3</v>
-      </c>
-      <c r="E40" s="99" t="s">
-        <v>175</v>
-      </c>
-      <c r="F40" s="96" t="s">
-        <v>169</v>
-      </c>
-      <c r="G40" s="91"/>
-      <c r="H40" s="91"/>
-      <c r="I40" s="100" t="s">
-        <v>170</v>
-      </c>
-      <c r="J40" s="91"/>
-      <c r="K40" s="91"/>
-      <c r="L40" s="91"/>
-      <c r="M40" s="91"/>
-      <c r="N40" s="91"/>
-      <c r="O40" s="91"/>
-      <c r="P40" s="91"/>
-      <c r="Q40" s="91"/>
-      <c r="R40" s="91"/>
-      <c r="S40" s="91"/>
-      <c r="T40" s="91"/>
-      <c r="U40" s="91"/>
-      <c r="V40" s="91"/>
-      <c r="W40" s="91"/>
-      <c r="X40" s="91"/>
-      <c r="Y40" s="91"/>
-      <c r="Z40" s="91"/>
-      <c r="AA40" s="91"/>
-      <c r="AB40" s="91"/>
-      <c r="AC40" s="91"/>
-      <c r="AD40" s="91"/>
-      <c r="AE40" s="91"/>
-      <c r="AF40" s="91"/>
-      <c r="AG40" s="91"/>
-      <c r="AH40" s="91"/>
-      <c r="AI40" s="91"/>
-      <c r="AJ40" s="91"/>
-      <c r="AK40" s="91"/>
-      <c r="AL40" s="91"/>
-      <c r="AM40" s="91"/>
-      <c r="AN40" s="91"/>
-      <c r="AO40" s="91"/>
-      <c r="AP40" s="91"/>
-      <c r="AQ40" s="91"/>
-      <c r="AR40" s="91"/>
-      <c r="AS40" s="91"/>
-      <c r="AT40" s="91"/>
-      <c r="AU40" s="91"/>
-      <c r="AV40" s="91"/>
-      <c r="AW40" s="91"/>
-      <c r="AX40" s="91"/>
-      <c r="AY40" s="91"/>
-      <c r="AZ40" s="91"/>
-      <c r="BA40" s="91"/>
-      <c r="BB40" s="91"/>
-      <c r="BC40" s="91"/>
-      <c r="BD40" s="91"/>
-      <c r="BE40" s="91"/>
-      <c r="BF40" s="91"/>
-      <c r="BG40" s="91"/>
-      <c r="BH40" s="91"/>
-      <c r="BI40" s="91"/>
-      <c r="BJ40" s="91"/>
-      <c r="BK40" s="91"/>
-      <c r="BL40" s="91"/>
-      <c r="BM40" s="91"/>
-      <c r="BN40" s="91"/>
-      <c r="BO40" s="91"/>
-      <c r="BP40" s="91"/>
-      <c r="BQ40" s="91"/>
-      <c r="BR40" s="91"/>
-      <c r="BS40" s="91"/>
-      <c r="BT40" s="91"/>
-      <c r="BU40" s="91"/>
-      <c r="BV40" s="91"/>
-      <c r="BW40" s="91"/>
-      <c r="BX40" s="91"/>
-      <c r="BY40" s="91"/>
-      <c r="BZ40" s="91"/>
-      <c r="CA40" s="91"/>
-      <c r="CB40" s="91"/>
-      <c r="CC40" s="91"/>
-      <c r="CD40" s="91"/>
-      <c r="CE40" s="91"/>
-      <c r="CF40" s="91"/>
-      <c r="CG40" s="91"/>
-      <c r="CH40" s="91"/>
-      <c r="CI40" s="91"/>
-      <c r="CJ40" s="91"/>
-      <c r="CK40" s="91"/>
-      <c r="CL40" s="91"/>
-      <c r="CM40" s="91"/>
-      <c r="CN40" s="91"/>
-      <c r="CO40" s="91"/>
-      <c r="CP40" s="91"/>
-      <c r="CQ40" s="91"/>
-      <c r="CR40" s="91"/>
-      <c r="CS40" s="91"/>
-      <c r="CT40" s="91"/>
-      <c r="CU40" s="91"/>
-      <c r="CV40" s="91"/>
-      <c r="CW40" s="91"/>
-      <c r="CX40" s="91"/>
-      <c r="CY40" s="91"/>
-      <c r="CZ40" s="91"/>
-      <c r="DA40" s="91"/>
-      <c r="DB40" s="91"/>
-      <c r="DC40" s="91"/>
-      <c r="DD40" s="91"/>
-      <c r="DE40" s="91"/>
-      <c r="DF40" s="91"/>
-      <c r="DG40" s="91"/>
-      <c r="DH40" s="91"/>
-      <c r="DI40" s="91"/>
-      <c r="DJ40" s="91"/>
-      <c r="DK40" s="91"/>
-      <c r="DL40" s="91"/>
-      <c r="DM40" s="91"/>
-      <c r="DN40" s="91"/>
-      <c r="DO40" s="91"/>
-      <c r="DP40" s="91"/>
-      <c r="DQ40" s="91"/>
-      <c r="DR40" s="91"/>
-      <c r="DS40" s="91"/>
-      <c r="DT40" s="91"/>
-      <c r="DU40" s="91"/>
-      <c r="DV40" s="91"/>
-      <c r="DW40" s="91"/>
-      <c r="DX40" s="91"/>
-      <c r="DY40" s="91"/>
-      <c r="DZ40" s="91"/>
-      <c r="EA40" s="91"/>
-      <c r="EB40" s="91"/>
-      <c r="EC40" s="91"/>
-      <c r="ED40" s="91"/>
-      <c r="EE40" s="91"/>
-      <c r="EF40" s="91"/>
-      <c r="EG40" s="91"/>
-      <c r="EH40" s="91"/>
-      <c r="EI40" s="91"/>
-      <c r="EJ40" s="91"/>
-      <c r="EK40" s="91"/>
-      <c r="EL40" s="91"/>
-      <c r="EM40" s="91"/>
-      <c r="EN40" s="91"/>
-      <c r="EO40" s="91"/>
-      <c r="EP40" s="91"/>
-      <c r="EQ40" s="91"/>
-      <c r="ER40" s="91"/>
-      <c r="ES40" s="91"/>
-      <c r="ET40" s="91"/>
-      <c r="EU40" s="91"/>
-      <c r="EV40" s="91"/>
-      <c r="EW40" s="91"/>
-      <c r="EX40" s="91"/>
-      <c r="EY40" s="91"/>
-      <c r="EZ40" s="91"/>
-      <c r="FA40" s="91"/>
-      <c r="FB40" s="91"/>
-      <c r="FC40" s="91"/>
-      <c r="FD40" s="91"/>
-      <c r="FE40" s="91"/>
-      <c r="FF40" s="91"/>
-      <c r="FG40" s="91"/>
-      <c r="FH40" s="91"/>
-      <c r="FI40" s="91"/>
-      <c r="FJ40" s="91"/>
-      <c r="FK40" s="91"/>
-      <c r="FL40" s="91"/>
-      <c r="FM40" s="91"/>
-      <c r="FN40" s="91"/>
-      <c r="FO40" s="91"/>
-      <c r="FP40" s="91"/>
-      <c r="FQ40" s="91"/>
-      <c r="FR40" s="91"/>
-      <c r="FS40" s="91"/>
-      <c r="FT40" s="91"/>
-      <c r="FU40" s="91"/>
-      <c r="FV40" s="91"/>
-      <c r="FW40" s="91"/>
-      <c r="FX40" s="91"/>
-      <c r="FY40" s="91"/>
-      <c r="FZ40" s="91"/>
-      <c r="GA40" s="91"/>
-      <c r="GB40" s="91"/>
-      <c r="GC40" s="91"/>
-      <c r="GD40" s="91"/>
-      <c r="GE40" s="91"/>
-      <c r="GF40" s="91"/>
-      <c r="GG40" s="91"/>
-      <c r="GH40" s="91"/>
-      <c r="GI40" s="91"/>
-      <c r="GJ40" s="91"/>
-      <c r="GK40" s="91"/>
-      <c r="GL40" s="91"/>
-      <c r="GM40" s="91"/>
-      <c r="GN40" s="91"/>
-      <c r="GO40" s="91"/>
-      <c r="GP40" s="91"/>
-      <c r="GQ40" s="91"/>
-      <c r="GR40" s="91"/>
-      <c r="GS40" s="91"/>
-      <c r="GT40" s="91"/>
-      <c r="GU40" s="91"/>
-      <c r="GV40" s="91"/>
-      <c r="GW40" s="91"/>
-      <c r="GX40" s="91"/>
-      <c r="GY40" s="91"/>
-      <c r="GZ40" s="91"/>
-      <c r="HA40" s="91"/>
-      <c r="HB40" s="91"/>
-      <c r="HC40" s="91"/>
-      <c r="HD40" s="91"/>
-      <c r="HE40" s="91"/>
-      <c r="HF40" s="91"/>
-      <c r="HG40" s="91"/>
-      <c r="HH40" s="91"/>
-      <c r="HI40" s="91"/>
-      <c r="HJ40" s="91"/>
-      <c r="HK40" s="91"/>
-      <c r="HL40" s="91"/>
-      <c r="HM40" s="91"/>
-      <c r="HN40" s="91"/>
-      <c r="HO40" s="91"/>
-      <c r="HP40" s="91"/>
-      <c r="HQ40" s="91"/>
-      <c r="HR40" s="91"/>
-      <c r="HS40" s="91"/>
-      <c r="HT40" s="91"/>
-      <c r="HU40" s="91"/>
-      <c r="HV40" s="91"/>
-      <c r="HW40" s="91"/>
-      <c r="HX40" s="91"/>
-      <c r="HY40" s="91"/>
-      <c r="HZ40" s="91"/>
-      <c r="IA40" s="91"/>
-      <c r="IB40" s="91"/>
-      <c r="IC40" s="91"/>
-      <c r="ID40" s="91"/>
-      <c r="IE40" s="91"/>
-      <c r="IF40" s="91"/>
-      <c r="IG40" s="91"/>
-      <c r="IH40" s="91"/>
-      <c r="II40" s="91"/>
-      <c r="IJ40" s="91"/>
-      <c r="IK40" s="91"/>
-      <c r="IL40" s="91"/>
-      <c r="IM40" s="91"/>
-      <c r="IN40" s="91"/>
-      <c r="IO40" s="91"/>
-      <c r="IP40" s="91"/>
-      <c r="IQ40" s="91"/>
-      <c r="IR40" s="91"/>
-      <c r="IS40" s="91"/>
-      <c r="IT40" s="91"/>
-      <c r="IU40" s="91"/>
-      <c r="IV40" s="91"/>
-    </row>
-    <row r="41" spans="1:256" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E38" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J38" s="29"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
+    </row>
+    <row r="39" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="17">
+        <v>27</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="19">
+        <v>1</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="20"/>
+      <c r="I39" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J39" s="29"/>
+      <c r="K39" s="65"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="3"/>
+    </row>
+    <row r="40" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="17">
+        <v>28</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="19">
+        <v>1</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="20"/>
+      <c r="I40" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J40" s="29"/>
+      <c r="K40" s="65"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="3"/>
+    </row>
+    <row r="41" spans="1:256" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="92" t="s">
         <v>166</v>
       </c>
-      <c r="B41" s="93"/>
+      <c r="B41" s="93">
+        <v>29</v>
+      </c>
       <c r="C41" s="94" t="s">
-        <v>176</v>
-      </c>
-      <c r="D41" s="98">
-        <v>4</v>
-      </c>
-      <c r="E41" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="F41" s="99" t="s">
-        <v>179</v>
-      </c>
-      <c r="G41" s="91"/>
-      <c r="H41" s="91"/>
-      <c r="I41" s="100" t="s">
+        <v>167</v>
+      </c>
+      <c r="D41" s="95">
+        <v>1</v>
+      </c>
+      <c r="E41" s="96" t="s">
+        <v>171</v>
+      </c>
+      <c r="F41" s="96" t="s">
+        <v>172</v>
+      </c>
+      <c r="G41" s="101"/>
+      <c r="H41" s="99"/>
+      <c r="I41" s="97" t="s">
         <v>170</v>
       </c>
-      <c r="J41" s="91"/>
-      <c r="K41" s="91"/>
-      <c r="L41" s="91"/>
-      <c r="M41" s="91"/>
-      <c r="N41" s="91"/>
-      <c r="O41" s="91"/>
-      <c r="P41" s="91"/>
-      <c r="Q41" s="91"/>
-      <c r="R41" s="91"/>
-      <c r="S41" s="91"/>
-      <c r="T41" s="91"/>
+      <c r="J41" s="108" t="s">
+        <v>187</v>
+      </c>
+      <c r="K41" s="102"/>
+      <c r="L41" s="103"/>
+      <c r="M41" s="103"/>
+      <c r="N41" s="103"/>
+      <c r="O41" s="103"/>
+      <c r="P41" s="103"/>
+      <c r="Q41" s="103"/>
+      <c r="R41" s="103"/>
+      <c r="S41" s="103"/>
+      <c r="T41" s="103"/>
       <c r="U41" s="91"/>
       <c r="V41" s="91"/>
       <c r="W41" s="91"/>
@@ -6813,62 +7225,636 @@
       <c r="IU41" s="91"/>
       <c r="IV41" s="91"/>
     </row>
-    <row r="42" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:256" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="92" t="s">
-        <v>163</v>
-      </c>
-      <c r="B42" s="93">
-        <v>26</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="B42" s="93"/>
       <c r="C42" s="94" t="s">
-        <v>164</v>
-      </c>
-      <c r="D42" s="98">
-        <v>1</v>
-      </c>
-      <c r="E42" s="99" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="I42" s="100" t="s">
+        <v>178</v>
+      </c>
+      <c r="D42" s="95">
+        <v>2</v>
+      </c>
+      <c r="E42" s="96" t="s">
+        <v>168</v>
+      </c>
+      <c r="F42" s="96" t="s">
+        <v>173</v>
+      </c>
+      <c r="I42" s="97" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="43" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J42" s="108" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="43" spans="1:256" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="92" t="s">
-        <v>163</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="B43" s="93"/>
       <c r="C43" s="94" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D43" s="98">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E43" s="99" t="s">
-        <v>165</v>
-      </c>
-      <c r="F43" s="99" t="s">
-        <v>181</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="F43" s="96" t="s">
+        <v>169</v>
+      </c>
+      <c r="G43" s="91"/>
+      <c r="H43" s="91"/>
       <c r="I43" s="100" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="44" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="94" t="s">
+      <c r="J43" s="108" t="s">
+        <v>187</v>
+      </c>
+      <c r="K43" s="91"/>
+      <c r="L43" s="91"/>
+      <c r="M43" s="91"/>
+      <c r="N43" s="91"/>
+      <c r="O43" s="91"/>
+      <c r="P43" s="91"/>
+      <c r="Q43" s="91"/>
+      <c r="R43" s="91"/>
+      <c r="S43" s="91"/>
+      <c r="T43" s="91"/>
+      <c r="U43" s="91"/>
+      <c r="V43" s="91"/>
+      <c r="W43" s="91"/>
+      <c r="X43" s="91"/>
+      <c r="Y43" s="91"/>
+      <c r="Z43" s="91"/>
+      <c r="AA43" s="91"/>
+      <c r="AB43" s="91"/>
+      <c r="AC43" s="91"/>
+      <c r="AD43" s="91"/>
+      <c r="AE43" s="91"/>
+      <c r="AF43" s="91"/>
+      <c r="AG43" s="91"/>
+      <c r="AH43" s="91"/>
+      <c r="AI43" s="91"/>
+      <c r="AJ43" s="91"/>
+      <c r="AK43" s="91"/>
+      <c r="AL43" s="91"/>
+      <c r="AM43" s="91"/>
+      <c r="AN43" s="91"/>
+      <c r="AO43" s="91"/>
+      <c r="AP43" s="91"/>
+      <c r="AQ43" s="91"/>
+      <c r="AR43" s="91"/>
+      <c r="AS43" s="91"/>
+      <c r="AT43" s="91"/>
+      <c r="AU43" s="91"/>
+      <c r="AV43" s="91"/>
+      <c r="AW43" s="91"/>
+      <c r="AX43" s="91"/>
+      <c r="AY43" s="91"/>
+      <c r="AZ43" s="91"/>
+      <c r="BA43" s="91"/>
+      <c r="BB43" s="91"/>
+      <c r="BC43" s="91"/>
+      <c r="BD43" s="91"/>
+      <c r="BE43" s="91"/>
+      <c r="BF43" s="91"/>
+      <c r="BG43" s="91"/>
+      <c r="BH43" s="91"/>
+      <c r="BI43" s="91"/>
+      <c r="BJ43" s="91"/>
+      <c r="BK43" s="91"/>
+      <c r="BL43" s="91"/>
+      <c r="BM43" s="91"/>
+      <c r="BN43" s="91"/>
+      <c r="BO43" s="91"/>
+      <c r="BP43" s="91"/>
+      <c r="BQ43" s="91"/>
+      <c r="BR43" s="91"/>
+      <c r="BS43" s="91"/>
+      <c r="BT43" s="91"/>
+      <c r="BU43" s="91"/>
+      <c r="BV43" s="91"/>
+      <c r="BW43" s="91"/>
+      <c r="BX43" s="91"/>
+      <c r="BY43" s="91"/>
+      <c r="BZ43" s="91"/>
+      <c r="CA43" s="91"/>
+      <c r="CB43" s="91"/>
+      <c r="CC43" s="91"/>
+      <c r="CD43" s="91"/>
+      <c r="CE43" s="91"/>
+      <c r="CF43" s="91"/>
+      <c r="CG43" s="91"/>
+      <c r="CH43" s="91"/>
+      <c r="CI43" s="91"/>
+      <c r="CJ43" s="91"/>
+      <c r="CK43" s="91"/>
+      <c r="CL43" s="91"/>
+      <c r="CM43" s="91"/>
+      <c r="CN43" s="91"/>
+      <c r="CO43" s="91"/>
+      <c r="CP43" s="91"/>
+      <c r="CQ43" s="91"/>
+      <c r="CR43" s="91"/>
+      <c r="CS43" s="91"/>
+      <c r="CT43" s="91"/>
+      <c r="CU43" s="91"/>
+      <c r="CV43" s="91"/>
+      <c r="CW43" s="91"/>
+      <c r="CX43" s="91"/>
+      <c r="CY43" s="91"/>
+      <c r="CZ43" s="91"/>
+      <c r="DA43" s="91"/>
+      <c r="DB43" s="91"/>
+      <c r="DC43" s="91"/>
+      <c r="DD43" s="91"/>
+      <c r="DE43" s="91"/>
+      <c r="DF43" s="91"/>
+      <c r="DG43" s="91"/>
+      <c r="DH43" s="91"/>
+      <c r="DI43" s="91"/>
+      <c r="DJ43" s="91"/>
+      <c r="DK43" s="91"/>
+      <c r="DL43" s="91"/>
+      <c r="DM43" s="91"/>
+      <c r="DN43" s="91"/>
+      <c r="DO43" s="91"/>
+      <c r="DP43" s="91"/>
+      <c r="DQ43" s="91"/>
+      <c r="DR43" s="91"/>
+      <c r="DS43" s="91"/>
+      <c r="DT43" s="91"/>
+      <c r="DU43" s="91"/>
+      <c r="DV43" s="91"/>
+      <c r="DW43" s="91"/>
+      <c r="DX43" s="91"/>
+      <c r="DY43" s="91"/>
+      <c r="DZ43" s="91"/>
+      <c r="EA43" s="91"/>
+      <c r="EB43" s="91"/>
+      <c r="EC43" s="91"/>
+      <c r="ED43" s="91"/>
+      <c r="EE43" s="91"/>
+      <c r="EF43" s="91"/>
+      <c r="EG43" s="91"/>
+      <c r="EH43" s="91"/>
+      <c r="EI43" s="91"/>
+      <c r="EJ43" s="91"/>
+      <c r="EK43" s="91"/>
+      <c r="EL43" s="91"/>
+      <c r="EM43" s="91"/>
+      <c r="EN43" s="91"/>
+      <c r="EO43" s="91"/>
+      <c r="EP43" s="91"/>
+      <c r="EQ43" s="91"/>
+      <c r="ER43" s="91"/>
+      <c r="ES43" s="91"/>
+      <c r="ET43" s="91"/>
+      <c r="EU43" s="91"/>
+      <c r="EV43" s="91"/>
+      <c r="EW43" s="91"/>
+      <c r="EX43" s="91"/>
+      <c r="EY43" s="91"/>
+      <c r="EZ43" s="91"/>
+      <c r="FA43" s="91"/>
+      <c r="FB43" s="91"/>
+      <c r="FC43" s="91"/>
+      <c r="FD43" s="91"/>
+      <c r="FE43" s="91"/>
+      <c r="FF43" s="91"/>
+      <c r="FG43" s="91"/>
+      <c r="FH43" s="91"/>
+      <c r="FI43" s="91"/>
+      <c r="FJ43" s="91"/>
+      <c r="FK43" s="91"/>
+      <c r="FL43" s="91"/>
+      <c r="FM43" s="91"/>
+      <c r="FN43" s="91"/>
+      <c r="FO43" s="91"/>
+      <c r="FP43" s="91"/>
+      <c r="FQ43" s="91"/>
+      <c r="FR43" s="91"/>
+      <c r="FS43" s="91"/>
+      <c r="FT43" s="91"/>
+      <c r="FU43" s="91"/>
+      <c r="FV43" s="91"/>
+      <c r="FW43" s="91"/>
+      <c r="FX43" s="91"/>
+      <c r="FY43" s="91"/>
+      <c r="FZ43" s="91"/>
+      <c r="GA43" s="91"/>
+      <c r="GB43" s="91"/>
+      <c r="GC43" s="91"/>
+      <c r="GD43" s="91"/>
+      <c r="GE43" s="91"/>
+      <c r="GF43" s="91"/>
+      <c r="GG43" s="91"/>
+      <c r="GH43" s="91"/>
+      <c r="GI43" s="91"/>
+      <c r="GJ43" s="91"/>
+      <c r="GK43" s="91"/>
+      <c r="GL43" s="91"/>
+      <c r="GM43" s="91"/>
+      <c r="GN43" s="91"/>
+      <c r="GO43" s="91"/>
+      <c r="GP43" s="91"/>
+      <c r="GQ43" s="91"/>
+      <c r="GR43" s="91"/>
+      <c r="GS43" s="91"/>
+      <c r="GT43" s="91"/>
+      <c r="GU43" s="91"/>
+      <c r="GV43" s="91"/>
+      <c r="GW43" s="91"/>
+      <c r="GX43" s="91"/>
+      <c r="GY43" s="91"/>
+      <c r="GZ43" s="91"/>
+      <c r="HA43" s="91"/>
+      <c r="HB43" s="91"/>
+      <c r="HC43" s="91"/>
+      <c r="HD43" s="91"/>
+      <c r="HE43" s="91"/>
+      <c r="HF43" s="91"/>
+      <c r="HG43" s="91"/>
+      <c r="HH43" s="91"/>
+      <c r="HI43" s="91"/>
+      <c r="HJ43" s="91"/>
+      <c r="HK43" s="91"/>
+      <c r="HL43" s="91"/>
+      <c r="HM43" s="91"/>
+      <c r="HN43" s="91"/>
+      <c r="HO43" s="91"/>
+      <c r="HP43" s="91"/>
+      <c r="HQ43" s="91"/>
+      <c r="HR43" s="91"/>
+      <c r="HS43" s="91"/>
+      <c r="HT43" s="91"/>
+      <c r="HU43" s="91"/>
+      <c r="HV43" s="91"/>
+      <c r="HW43" s="91"/>
+      <c r="HX43" s="91"/>
+      <c r="HY43" s="91"/>
+      <c r="HZ43" s="91"/>
+      <c r="IA43" s="91"/>
+      <c r="IB43" s="91"/>
+      <c r="IC43" s="91"/>
+      <c r="ID43" s="91"/>
+      <c r="IE43" s="91"/>
+      <c r="IF43" s="91"/>
+      <c r="IG43" s="91"/>
+      <c r="IH43" s="91"/>
+      <c r="II43" s="91"/>
+      <c r="IJ43" s="91"/>
+      <c r="IK43" s="91"/>
+      <c r="IL43" s="91"/>
+      <c r="IM43" s="91"/>
+      <c r="IN43" s="91"/>
+      <c r="IO43" s="91"/>
+      <c r="IP43" s="91"/>
+      <c r="IQ43" s="91"/>
+      <c r="IR43" s="91"/>
+      <c r="IS43" s="91"/>
+      <c r="IT43" s="91"/>
+      <c r="IU43" s="91"/>
+      <c r="IV43" s="91"/>
+    </row>
+    <row r="44" spans="1:256" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="92" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" s="93"/>
+      <c r="C44" s="94" t="s">
+        <v>176</v>
+      </c>
+      <c r="D44" s="98">
+        <v>4</v>
+      </c>
+      <c r="E44" s="99" t="s">
+        <v>177</v>
+      </c>
+      <c r="F44" s="99" t="s">
+        <v>179</v>
+      </c>
+      <c r="G44" s="91"/>
+      <c r="H44" s="91"/>
+      <c r="I44" s="100" t="s">
+        <v>170</v>
+      </c>
+      <c r="J44" s="108" t="s">
+        <v>187</v>
+      </c>
+      <c r="K44" s="91"/>
+      <c r="L44" s="91"/>
+      <c r="M44" s="91"/>
+      <c r="N44" s="91"/>
+      <c r="O44" s="91"/>
+      <c r="P44" s="91"/>
+      <c r="Q44" s="91"/>
+      <c r="R44" s="91"/>
+      <c r="S44" s="91"/>
+      <c r="T44" s="91"/>
+      <c r="U44" s="91"/>
+      <c r="V44" s="91"/>
+      <c r="W44" s="91"/>
+      <c r="X44" s="91"/>
+      <c r="Y44" s="91"/>
+      <c r="Z44" s="91"/>
+      <c r="AA44" s="91"/>
+      <c r="AB44" s="91"/>
+      <c r="AC44" s="91"/>
+      <c r="AD44" s="91"/>
+      <c r="AE44" s="91"/>
+      <c r="AF44" s="91"/>
+      <c r="AG44" s="91"/>
+      <c r="AH44" s="91"/>
+      <c r="AI44" s="91"/>
+      <c r="AJ44" s="91"/>
+      <c r="AK44" s="91"/>
+      <c r="AL44" s="91"/>
+      <c r="AM44" s="91"/>
+      <c r="AN44" s="91"/>
+      <c r="AO44" s="91"/>
+      <c r="AP44" s="91"/>
+      <c r="AQ44" s="91"/>
+      <c r="AR44" s="91"/>
+      <c r="AS44" s="91"/>
+      <c r="AT44" s="91"/>
+      <c r="AU44" s="91"/>
+      <c r="AV44" s="91"/>
+      <c r="AW44" s="91"/>
+      <c r="AX44" s="91"/>
+      <c r="AY44" s="91"/>
+      <c r="AZ44" s="91"/>
+      <c r="BA44" s="91"/>
+      <c r="BB44" s="91"/>
+      <c r="BC44" s="91"/>
+      <c r="BD44" s="91"/>
+      <c r="BE44" s="91"/>
+      <c r="BF44" s="91"/>
+      <c r="BG44" s="91"/>
+      <c r="BH44" s="91"/>
+      <c r="BI44" s="91"/>
+      <c r="BJ44" s="91"/>
+      <c r="BK44" s="91"/>
+      <c r="BL44" s="91"/>
+      <c r="BM44" s="91"/>
+      <c r="BN44" s="91"/>
+      <c r="BO44" s="91"/>
+      <c r="BP44" s="91"/>
+      <c r="BQ44" s="91"/>
+      <c r="BR44" s="91"/>
+      <c r="BS44" s="91"/>
+      <c r="BT44" s="91"/>
+      <c r="BU44" s="91"/>
+      <c r="BV44" s="91"/>
+      <c r="BW44" s="91"/>
+      <c r="BX44" s="91"/>
+      <c r="BY44" s="91"/>
+      <c r="BZ44" s="91"/>
+      <c r="CA44" s="91"/>
+      <c r="CB44" s="91"/>
+      <c r="CC44" s="91"/>
+      <c r="CD44" s="91"/>
+      <c r="CE44" s="91"/>
+      <c r="CF44" s="91"/>
+      <c r="CG44" s="91"/>
+      <c r="CH44" s="91"/>
+      <c r="CI44" s="91"/>
+      <c r="CJ44" s="91"/>
+      <c r="CK44" s="91"/>
+      <c r="CL44" s="91"/>
+      <c r="CM44" s="91"/>
+      <c r="CN44" s="91"/>
+      <c r="CO44" s="91"/>
+      <c r="CP44" s="91"/>
+      <c r="CQ44" s="91"/>
+      <c r="CR44" s="91"/>
+      <c r="CS44" s="91"/>
+      <c r="CT44" s="91"/>
+      <c r="CU44" s="91"/>
+      <c r="CV44" s="91"/>
+      <c r="CW44" s="91"/>
+      <c r="CX44" s="91"/>
+      <c r="CY44" s="91"/>
+      <c r="CZ44" s="91"/>
+      <c r="DA44" s="91"/>
+      <c r="DB44" s="91"/>
+      <c r="DC44" s="91"/>
+      <c r="DD44" s="91"/>
+      <c r="DE44" s="91"/>
+      <c r="DF44" s="91"/>
+      <c r="DG44" s="91"/>
+      <c r="DH44" s="91"/>
+      <c r="DI44" s="91"/>
+      <c r="DJ44" s="91"/>
+      <c r="DK44" s="91"/>
+      <c r="DL44" s="91"/>
+      <c r="DM44" s="91"/>
+      <c r="DN44" s="91"/>
+      <c r="DO44" s="91"/>
+      <c r="DP44" s="91"/>
+      <c r="DQ44" s="91"/>
+      <c r="DR44" s="91"/>
+      <c r="DS44" s="91"/>
+      <c r="DT44" s="91"/>
+      <c r="DU44" s="91"/>
+      <c r="DV44" s="91"/>
+      <c r="DW44" s="91"/>
+      <c r="DX44" s="91"/>
+      <c r="DY44" s="91"/>
+      <c r="DZ44" s="91"/>
+      <c r="EA44" s="91"/>
+      <c r="EB44" s="91"/>
+      <c r="EC44" s="91"/>
+      <c r="ED44" s="91"/>
+      <c r="EE44" s="91"/>
+      <c r="EF44" s="91"/>
+      <c r="EG44" s="91"/>
+      <c r="EH44" s="91"/>
+      <c r="EI44" s="91"/>
+      <c r="EJ44" s="91"/>
+      <c r="EK44" s="91"/>
+      <c r="EL44" s="91"/>
+      <c r="EM44" s="91"/>
+      <c r="EN44" s="91"/>
+      <c r="EO44" s="91"/>
+      <c r="EP44" s="91"/>
+      <c r="EQ44" s="91"/>
+      <c r="ER44" s="91"/>
+      <c r="ES44" s="91"/>
+      <c r="ET44" s="91"/>
+      <c r="EU44" s="91"/>
+      <c r="EV44" s="91"/>
+      <c r="EW44" s="91"/>
+      <c r="EX44" s="91"/>
+      <c r="EY44" s="91"/>
+      <c r="EZ44" s="91"/>
+      <c r="FA44" s="91"/>
+      <c r="FB44" s="91"/>
+      <c r="FC44" s="91"/>
+      <c r="FD44" s="91"/>
+      <c r="FE44" s="91"/>
+      <c r="FF44" s="91"/>
+      <c r="FG44" s="91"/>
+      <c r="FH44" s="91"/>
+      <c r="FI44" s="91"/>
+      <c r="FJ44" s="91"/>
+      <c r="FK44" s="91"/>
+      <c r="FL44" s="91"/>
+      <c r="FM44" s="91"/>
+      <c r="FN44" s="91"/>
+      <c r="FO44" s="91"/>
+      <c r="FP44" s="91"/>
+      <c r="FQ44" s="91"/>
+      <c r="FR44" s="91"/>
+      <c r="FS44" s="91"/>
+      <c r="FT44" s="91"/>
+      <c r="FU44" s="91"/>
+      <c r="FV44" s="91"/>
+      <c r="FW44" s="91"/>
+      <c r="FX44" s="91"/>
+      <c r="FY44" s="91"/>
+      <c r="FZ44" s="91"/>
+      <c r="GA44" s="91"/>
+      <c r="GB44" s="91"/>
+      <c r="GC44" s="91"/>
+      <c r="GD44" s="91"/>
+      <c r="GE44" s="91"/>
+      <c r="GF44" s="91"/>
+      <c r="GG44" s="91"/>
+      <c r="GH44" s="91"/>
+      <c r="GI44" s="91"/>
+      <c r="GJ44" s="91"/>
+      <c r="GK44" s="91"/>
+      <c r="GL44" s="91"/>
+      <c r="GM44" s="91"/>
+      <c r="GN44" s="91"/>
+      <c r="GO44" s="91"/>
+      <c r="GP44" s="91"/>
+      <c r="GQ44" s="91"/>
+      <c r="GR44" s="91"/>
+      <c r="GS44" s="91"/>
+      <c r="GT44" s="91"/>
+      <c r="GU44" s="91"/>
+      <c r="GV44" s="91"/>
+      <c r="GW44" s="91"/>
+      <c r="GX44" s="91"/>
+      <c r="GY44" s="91"/>
+      <c r="GZ44" s="91"/>
+      <c r="HA44" s="91"/>
+      <c r="HB44" s="91"/>
+      <c r="HC44" s="91"/>
+      <c r="HD44" s="91"/>
+      <c r="HE44" s="91"/>
+      <c r="HF44" s="91"/>
+      <c r="HG44" s="91"/>
+      <c r="HH44" s="91"/>
+      <c r="HI44" s="91"/>
+      <c r="HJ44" s="91"/>
+      <c r="HK44" s="91"/>
+      <c r="HL44" s="91"/>
+      <c r="HM44" s="91"/>
+      <c r="HN44" s="91"/>
+      <c r="HO44" s="91"/>
+      <c r="HP44" s="91"/>
+      <c r="HQ44" s="91"/>
+      <c r="HR44" s="91"/>
+      <c r="HS44" s="91"/>
+      <c r="HT44" s="91"/>
+      <c r="HU44" s="91"/>
+      <c r="HV44" s="91"/>
+      <c r="HW44" s="91"/>
+      <c r="HX44" s="91"/>
+      <c r="HY44" s="91"/>
+      <c r="HZ44" s="91"/>
+      <c r="IA44" s="91"/>
+      <c r="IB44" s="91"/>
+      <c r="IC44" s="91"/>
+      <c r="ID44" s="91"/>
+      <c r="IE44" s="91"/>
+      <c r="IF44" s="91"/>
+      <c r="IG44" s="91"/>
+      <c r="IH44" s="91"/>
+      <c r="II44" s="91"/>
+      <c r="IJ44" s="91"/>
+      <c r="IK44" s="91"/>
+      <c r="IL44" s="91"/>
+      <c r="IM44" s="91"/>
+      <c r="IN44" s="91"/>
+      <c r="IO44" s="91"/>
+      <c r="IP44" s="91"/>
+      <c r="IQ44" s="91"/>
+      <c r="IR44" s="91"/>
+      <c r="IS44" s="91"/>
+      <c r="IT44" s="91"/>
+      <c r="IU44" s="91"/>
+      <c r="IV44" s="91"/>
+    </row>
+    <row r="45" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="92" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="93">
+        <v>30</v>
+      </c>
+      <c r="C45" s="94" t="s">
+        <v>164</v>
+      </c>
+      <c r="D45" s="98">
+        <v>1</v>
+      </c>
+      <c r="E45" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="99" t="s">
+        <v>78</v>
+      </c>
+      <c r="I45" s="100" t="s">
+        <v>170</v>
+      </c>
+      <c r="J45" s="108" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="92" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" s="94" t="s">
+        <v>180</v>
+      </c>
+      <c r="D46" s="98">
+        <v>2</v>
+      </c>
+      <c r="E46" s="99" t="s">
+        <v>165</v>
+      </c>
+      <c r="F46" s="99" t="s">
+        <v>181</v>
+      </c>
+      <c r="I46" s="100" t="s">
+        <v>170</v>
+      </c>
+      <c r="J46" s="108" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="94" t="s">
         <v>182</v>
       </c>
-      <c r="IV44"/>
+      <c r="IV47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update Homework Assignments/a15/CS 3398 Test Tracker.xlsx
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
+++ b/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NinoPinto\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE81A05-FFBD-4493-BD2B-74024EBF2730}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ED9F46-265E-4329-9BBE-A698F0A89156}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="217">
   <si>
     <t>Expectations</t>
   </si>
@@ -859,12 +859,14 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -876,6 +878,7 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4682,8 +4685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6975,9 +6978,7 @@
       <c r="I41" s="97" t="s">
         <v>170</v>
       </c>
-      <c r="J41" s="108" t="s">
-        <v>187</v>
-      </c>
+      <c r="J41" s="108"/>
       <c r="K41" s="102"/>
       <c r="L41" s="103"/>
       <c r="M41" s="103"/>
@@ -7245,9 +7246,7 @@
       <c r="I42" s="97" t="s">
         <v>170</v>
       </c>
-      <c r="J42" s="108" t="s">
-        <v>187</v>
-      </c>
+      <c r="J42" s="108"/>
     </row>
     <row r="43" spans="1:256" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="92" t="s">
@@ -7271,9 +7270,7 @@
       <c r="I43" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="J43" s="108" t="s">
-        <v>187</v>
-      </c>
+      <c r="J43" s="108"/>
       <c r="K43" s="91"/>
       <c r="L43" s="91"/>
       <c r="M43" s="91"/>
@@ -7543,9 +7540,7 @@
       <c r="I44" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="J44" s="108" t="s">
-        <v>187</v>
-      </c>
+      <c r="J44" s="108"/>
       <c r="K44" s="91"/>
       <c r="L44" s="91"/>
       <c r="M44" s="91"/>
@@ -7815,9 +7810,7 @@
       <c r="I45" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="J45" s="108" t="s">
-        <v>187</v>
-      </c>
+      <c r="J45" s="108"/>
     </row>
     <row r="46" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="92" t="s">
@@ -7838,9 +7831,7 @@
       <c r="I46" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="J46" s="108" t="s">
-        <v>187</v>
-      </c>
+      <c r="J46" s="108"/>
     </row>
     <row r="47" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="94" t="s">

</xml_diff>

<commit_message>
Added screenshots for Eric's tests
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
+++ b/Homework Assignments/a15/CS 3398 Test Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NinoPinto\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6203C4B0-4378-4510-84B3-D45FD9471206}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D6959C-76E5-4681-B4C9-66BF6AA38D18}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17565" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="224">
   <si>
     <t>Expectations</t>
   </si>
@@ -844,6 +844,24 @@
   </si>
   <si>
     <t>Bot does not recognize video ID as valid</t>
+  </si>
+  <si>
+    <t>Works perfect, decrements and increments right amount</t>
+  </si>
+  <si>
+    <t>Bot causes an error with the hug count, shows NaN hugs instead of 0</t>
+  </si>
+  <si>
+    <t>Connects</t>
+  </si>
+  <si>
+    <t>Shows correct hugs</t>
+  </si>
+  <si>
+    <t>Increments/Decrements correctly</t>
+  </si>
+  <si>
+    <t>Works perfect</t>
   </si>
 </sst>
 </file>
@@ -4688,8 +4706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6617,11 +6635,15 @@
       <c r="G31" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="20"/>
+      <c r="H31" s="20" t="s">
+        <v>220</v>
+      </c>
       <c r="I31" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="J31" s="29"/>
+      <c r="J31" s="29" t="s">
+        <v>187</v>
+      </c>
       <c r="K31" s="65"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -6651,7 +6673,9 @@
       <c r="G32" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="20"/>
+      <c r="H32" s="20" t="s">
+        <v>221</v>
+      </c>
       <c r="I32" s="23" t="s">
         <v>79</v>
       </c>
@@ -6685,7 +6709,9 @@
       <c r="G33" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="20"/>
+      <c r="H33" s="20" t="s">
+        <v>221</v>
+      </c>
       <c r="I33" s="23" t="s">
         <v>79</v>
       </c>
@@ -6723,11 +6749,15 @@
       <c r="G34" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H34" s="20"/>
+      <c r="H34" s="20" t="s">
+        <v>220</v>
+      </c>
       <c r="I34" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="J34" s="29"/>
+      <c r="J34" s="29" t="s">
+        <v>187</v>
+      </c>
       <c r="K34" s="65"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -6757,7 +6787,9 @@
       <c r="G35" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H35" s="20"/>
+      <c r="H35" s="20" t="s">
+        <v>222</v>
+      </c>
       <c r="I35" s="23" t="s">
         <v>79</v>
       </c>
@@ -6791,7 +6823,9 @@
       <c r="G36" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="H36" s="20"/>
+      <c r="H36" s="20" t="s">
+        <v>219</v>
+      </c>
       <c r="I36" s="23" t="s">
         <v>79</v>
       </c>
@@ -6829,11 +6863,15 @@
       <c r="G37" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="20"/>
+      <c r="H37" s="20" t="s">
+        <v>218</v>
+      </c>
       <c r="I37" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="J37" s="29"/>
+      <c r="J37" s="29" t="s">
+        <v>187</v>
+      </c>
       <c r="K37" s="65"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -6873,7 +6911,9 @@
       <c r="I38" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="J38" s="29"/>
+      <c r="J38" s="29" t="s">
+        <v>187</v>
+      </c>
       <c r="K38" s="65"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -6907,11 +6947,15 @@
       <c r="G39" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H39" s="20"/>
+      <c r="H39" s="20" t="s">
+        <v>223</v>
+      </c>
       <c r="I39" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="J39" s="29"/>
+      <c r="J39" s="29" t="s">
+        <v>187</v>
+      </c>
       <c r="K39" s="65"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -6945,11 +6989,15 @@
       <c r="G40" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H40" s="20"/>
+      <c r="H40" s="20" t="s">
+        <v>223</v>
+      </c>
       <c r="I40" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="J40" s="29"/>
+      <c r="J40" s="29" t="s">
+        <v>187</v>
+      </c>
       <c r="K40" s="65"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
@@ -6985,7 +7033,9 @@
       <c r="I41" s="97" t="s">
         <v>170</v>
       </c>
-      <c r="J41" s="108"/>
+      <c r="J41" s="108" t="s">
+        <v>17</v>
+      </c>
       <c r="K41" s="102"/>
       <c r="L41" s="103"/>
       <c r="M41" s="103"/>
@@ -7253,7 +7303,9 @@
       <c r="I42" s="97" t="s">
         <v>170</v>
       </c>
-      <c r="J42" s="108"/>
+      <c r="J42" s="108" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="43" spans="1:256" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="92" t="s">
@@ -7277,7 +7329,9 @@
       <c r="I43" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="J43" s="108"/>
+      <c r="J43" s="108" t="s">
+        <v>17</v>
+      </c>
       <c r="K43" s="91"/>
       <c r="L43" s="91"/>
       <c r="M43" s="91"/>
@@ -7547,7 +7601,9 @@
       <c r="I44" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="J44" s="108"/>
+      <c r="J44" s="108" t="s">
+        <v>17</v>
+      </c>
       <c r="K44" s="91"/>
       <c r="L44" s="91"/>
       <c r="M44" s="91"/>
@@ -7817,7 +7873,9 @@
       <c r="I45" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="J45" s="108"/>
+      <c r="J45" s="108" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="46" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="92" t="s">
@@ -7838,7 +7896,9 @@
       <c r="I46" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="J46" s="108"/>
+      <c r="J46" s="108" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="47" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="94" t="s">

</xml_diff>